<commit_message>
Oops: forgot that not setting an ordinal end would prevent trailing extras
</commit_message>
<xml_diff>
--- a/math-decks/basic-arithmetic-number-sense/Card Types/{Data Sheet Chunk} 3. Basic Operations, Single Items.xlsx
+++ b/math-decks/basic-arithmetic-number-sense/Card Types/{Data Sheet Chunk} 3. Basic Operations, Single Items.xlsx
@@ -157,7 +157,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF0070C0"/>
@@ -189,8 +194,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="Table Style 1" pivot="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="2"/>
-      <tableStyleElement type="headerRow" dxfId="1"/>
+      <tableStyleElement type="wholeTable" dxfId="3"/>
+      <tableStyleElement type="headerRow" dxfId="2"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -578,6 +583,9 @@
       <c r="E3">
         <v>1</v>
       </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
       <c r="G3">
         <v>10</v>
       </c>
@@ -615,6 +623,9 @@
       <c r="E4">
         <v>2</v>
       </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
       <c r="G4">
         <v>10</v>
       </c>
@@ -651,6 +662,9 @@
       <c r="E5">
         <v>3</v>
       </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
       <c r="G5">
         <v>10</v>
       </c>
@@ -681,6 +695,9 @@
       <c r="E6">
         <v>4</v>
       </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
       <c r="G6">
         <v>10</v>
       </c>
@@ -717,6 +734,9 @@
       <c r="E7">
         <v>5</v>
       </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
       <c r="G7">
         <v>10</v>
       </c>
@@ -753,6 +773,9 @@
       <c r="E8">
         <v>6</v>
       </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
       <c r="G8">
         <v>10</v>
       </c>
@@ -789,6 +812,9 @@
       <c r="E9">
         <v>7</v>
       </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
       <c r="G9">
         <v>10</v>
       </c>
@@ -825,6 +851,9 @@
       <c r="E10">
         <v>8</v>
       </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
       <c r="G10">
         <v>10</v>
       </c>
@@ -861,6 +890,9 @@
       <c r="E11">
         <v>9</v>
       </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
       <c r="G11">
         <v>10</v>
       </c>
@@ -926,9 +958,9 @@
         <f>IF(ISNUMBER(E3), E3, "")</f>
         <v>1</v>
       </c>
-      <c r="F13" t="str">
+      <c r="F13">
         <f>IF(ISNUMBER(F3), F3, "")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G13">
         <f>IF(ISNUMBER(G3), G3, "")</f>
@@ -968,9 +1000,9 @@
         <f t="shared" ref="E14:G14" si="4">IF(ISNUMBER(E4), E4, "")</f>
         <v>2</v>
       </c>
-      <c r="F14" t="str">
+      <c r="F14">
         <f t="shared" si="4"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G14">
         <f t="shared" si="4"/>
@@ -1010,9 +1042,9 @@
         <f t="shared" ref="E15:G15" si="7">IF(ISNUMBER(E5), E5, "")</f>
         <v>3</v>
       </c>
-      <c r="F15" t="str">
+      <c r="F15">
         <f t="shared" si="7"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G15">
         <f t="shared" si="7"/>
@@ -1052,9 +1084,9 @@
         <f t="shared" ref="E16:G16" si="8">IF(ISNUMBER(E6), E6, "")</f>
         <v>4</v>
       </c>
-      <c r="F16" t="str">
+      <c r="F16">
         <f t="shared" si="8"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G16">
         <f t="shared" si="8"/>
@@ -1094,9 +1126,9 @@
         <f t="shared" ref="E17:G17" si="9">IF(ISNUMBER(E7), E7, "")</f>
         <v>5</v>
       </c>
-      <c r="F17" t="str">
+      <c r="F17">
         <f t="shared" si="9"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G17">
         <f t="shared" si="9"/>
@@ -1136,9 +1168,9 @@
         <f t="shared" ref="E18:G18" si="10">IF(ISNUMBER(E8), E8, "")</f>
         <v>6</v>
       </c>
-      <c r="F18" t="str">
+      <c r="F18">
         <f t="shared" si="10"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G18">
         <f t="shared" si="10"/>
@@ -1178,9 +1210,9 @@
         <f t="shared" ref="E19:G19" si="11">IF(ISNUMBER(E9), E9, "")</f>
         <v>7</v>
       </c>
-      <c r="F19" t="str">
+      <c r="F19">
         <f t="shared" si="11"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G19">
         <f t="shared" si="11"/>
@@ -1220,9 +1252,9 @@
         <f t="shared" ref="E20:G20" si="12">IF(ISNUMBER(E10), E10, "")</f>
         <v>8</v>
       </c>
-      <c r="F20" t="str">
+      <c r="F20">
         <f t="shared" si="12"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G20">
         <f t="shared" si="12"/>
@@ -1262,9 +1294,9 @@
         <f t="shared" ref="E21:G21" si="13">IF(ISNUMBER(E11), E11, "")</f>
         <v>9</v>
       </c>
-      <c r="F21" t="str">
+      <c r="F21">
         <f t="shared" si="13"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G21">
         <f t="shared" si="13"/>
@@ -1346,9 +1378,9 @@
         <f t="shared" ref="E23:G23" si="15">IF(ISNUMBER(E13), E13, "")</f>
         <v>1</v>
       </c>
-      <c r="F23" t="str">
+      <c r="F23">
         <f t="shared" si="15"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G23">
         <f t="shared" si="15"/>
@@ -1388,9 +1420,9 @@
         <f t="shared" ref="E24:G24" si="16">IF(ISNUMBER(E14), E14, "")</f>
         <v>2</v>
       </c>
-      <c r="F24" t="str">
+      <c r="F24">
         <f t="shared" si="16"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G24">
         <f t="shared" si="16"/>
@@ -1430,9 +1462,9 @@
         <f t="shared" ref="E25:G25" si="17">IF(ISNUMBER(E15), E15, "")</f>
         <v>3</v>
       </c>
-      <c r="F25" t="str">
+      <c r="F25">
         <f t="shared" si="17"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G25">
         <f t="shared" si="17"/>
@@ -1472,9 +1504,9 @@
         <f t="shared" ref="E26:G26" si="18">IF(ISNUMBER(E16), E16, "")</f>
         <v>4</v>
       </c>
-      <c r="F26" t="str">
+      <c r="F26">
         <f t="shared" si="18"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G26">
         <f t="shared" si="18"/>
@@ -1514,9 +1546,9 @@
         <f t="shared" ref="E27:G27" si="19">IF(ISNUMBER(E17), E17, "")</f>
         <v>5</v>
       </c>
-      <c r="F27" t="str">
+      <c r="F27">
         <f t="shared" si="19"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G27">
         <f t="shared" si="19"/>
@@ -1556,9 +1588,9 @@
         <f t="shared" ref="E28:G28" si="20">IF(ISNUMBER(E18), E18, "")</f>
         <v>6</v>
       </c>
-      <c r="F28" t="str">
+      <c r="F28">
         <f t="shared" si="20"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G28">
         <f t="shared" si="20"/>
@@ -1598,9 +1630,9 @@
         <f t="shared" ref="E29:G29" si="21">IF(ISNUMBER(E19), E19, "")</f>
         <v>7</v>
       </c>
-      <c r="F29" t="str">
+      <c r="F29">
         <f t="shared" si="21"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G29">
         <f t="shared" si="21"/>
@@ -1640,9 +1672,9 @@
         <f t="shared" ref="E30:G30" si="22">IF(ISNUMBER(E20), E20, "")</f>
         <v>8</v>
       </c>
-      <c r="F30" t="str">
+      <c r="F30">
         <f t="shared" si="22"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G30">
         <f t="shared" si="22"/>
@@ -1682,9 +1714,9 @@
         <f t="shared" ref="E31:G31" si="23">IF(ISNUMBER(E21), E21, "")</f>
         <v>9</v>
       </c>
-      <c r="F31" t="str">
+      <c r="F31">
         <f t="shared" si="23"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G31">
         <f t="shared" si="23"/>
@@ -1766,9 +1798,9 @@
         <f t="shared" ref="E33:G33" si="25">IF(ISNUMBER(E23), E23, "")</f>
         <v>1</v>
       </c>
-      <c r="F33" t="str">
+      <c r="F33">
         <f t="shared" si="25"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G33">
         <f t="shared" si="25"/>
@@ -1808,9 +1840,9 @@
         <f t="shared" ref="E34:G34" si="26">IF(ISNUMBER(E24), E24, "")</f>
         <v>2</v>
       </c>
-      <c r="F34" t="str">
+      <c r="F34">
         <f t="shared" si="26"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G34">
         <f t="shared" si="26"/>
@@ -1850,9 +1882,9 @@
         <f t="shared" ref="E35:G35" si="27">IF(ISNUMBER(E25), E25, "")</f>
         <v>3</v>
       </c>
-      <c r="F35" t="str">
+      <c r="F35">
         <f t="shared" si="27"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G35">
         <f t="shared" si="27"/>
@@ -1892,9 +1924,9 @@
         <f t="shared" ref="E36:G36" si="28">IF(ISNUMBER(E26), E26, "")</f>
         <v>4</v>
       </c>
-      <c r="F36" t="str">
+      <c r="F36">
         <f t="shared" si="28"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G36">
         <f t="shared" si="28"/>
@@ -1934,9 +1966,9 @@
         <f t="shared" ref="E37:G37" si="29">IF(ISNUMBER(E27), E27, "")</f>
         <v>5</v>
       </c>
-      <c r="F37" t="str">
+      <c r="F37">
         <f t="shared" si="29"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G37">
         <f t="shared" si="29"/>
@@ -1976,9 +2008,9 @@
         <f t="shared" ref="E38:G38" si="30">IF(ISNUMBER(E28), E28, "")</f>
         <v>6</v>
       </c>
-      <c r="F38" t="str">
+      <c r="F38">
         <f t="shared" si="30"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G38">
         <f t="shared" si="30"/>
@@ -2018,9 +2050,9 @@
         <f t="shared" ref="E39:G39" si="31">IF(ISNUMBER(E29), E29, "")</f>
         <v>7</v>
       </c>
-      <c r="F39" t="str">
+      <c r="F39">
         <f t="shared" si="31"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G39">
         <f t="shared" si="31"/>
@@ -2060,9 +2092,9 @@
         <f t="shared" ref="E40:G40" si="32">IF(ISNUMBER(E30), E30, "")</f>
         <v>8</v>
       </c>
-      <c r="F40" t="str">
+      <c r="F40">
         <f t="shared" si="32"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G40">
         <f t="shared" si="32"/>
@@ -2102,9 +2134,9 @@
         <f t="shared" ref="E41:G41" si="33">IF(ISNUMBER(E31), E31, "")</f>
         <v>9</v>
       </c>
-      <c r="F41" t="str">
+      <c r="F41">
         <f t="shared" si="33"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G41">
         <f t="shared" si="33"/>
@@ -2186,9 +2218,9 @@
         <f t="shared" ref="E43:G43" si="35">IF(ISNUMBER(E33), E33, "")</f>
         <v>1</v>
       </c>
-      <c r="F43" t="str">
+      <c r="F43">
         <f t="shared" si="35"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G43">
         <f t="shared" si="35"/>
@@ -2228,9 +2260,9 @@
         <f t="shared" ref="E44:G44" si="36">IF(ISNUMBER(E34), E34, "")</f>
         <v>2</v>
       </c>
-      <c r="F44" t="str">
+      <c r="F44">
         <f t="shared" si="36"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G44">
         <f t="shared" si="36"/>
@@ -2270,9 +2302,9 @@
         <f t="shared" ref="E45:G45" si="37">IF(ISNUMBER(E35), E35, "")</f>
         <v>3</v>
       </c>
-      <c r="F45" t="str">
+      <c r="F45">
         <f t="shared" si="37"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G45">
         <f t="shared" si="37"/>
@@ -2312,9 +2344,9 @@
         <f t="shared" ref="E46:G46" si="38">IF(ISNUMBER(E36), E36, "")</f>
         <v>4</v>
       </c>
-      <c r="F46" t="str">
+      <c r="F46">
         <f t="shared" si="38"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G46">
         <f t="shared" si="38"/>
@@ -2354,9 +2386,9 @@
         <f t="shared" ref="E47:G47" si="39">IF(ISNUMBER(E37), E37, "")</f>
         <v>5</v>
       </c>
-      <c r="F47" t="str">
+      <c r="F47">
         <f t="shared" si="39"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G47">
         <f t="shared" si="39"/>
@@ -2396,9 +2428,9 @@
         <f t="shared" ref="E48:G48" si="40">IF(ISNUMBER(E38), E38, "")</f>
         <v>6</v>
       </c>
-      <c r="F48" t="str">
+      <c r="F48">
         <f t="shared" si="40"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G48">
         <f t="shared" si="40"/>
@@ -2438,9 +2470,9 @@
         <f t="shared" ref="E49:G49" si="41">IF(ISNUMBER(E39), E39, "")</f>
         <v>7</v>
       </c>
-      <c r="F49" t="str">
+      <c r="F49">
         <f t="shared" si="41"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G49">
         <f t="shared" si="41"/>
@@ -2480,9 +2512,9 @@
         <f t="shared" ref="E50:G50" si="42">IF(ISNUMBER(E40), E40, "")</f>
         <v>8</v>
       </c>
-      <c r="F50" t="str">
+      <c r="F50">
         <f t="shared" si="42"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G50">
         <f t="shared" si="42"/>
@@ -2522,9 +2554,9 @@
         <f t="shared" ref="E51:G51" si="43">IF(ISNUMBER(E41), E41, "")</f>
         <v>9</v>
       </c>
-      <c r="F51" t="str">
+      <c r="F51">
         <f t="shared" si="43"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G51">
         <f t="shared" si="43"/>
@@ -2606,9 +2638,9 @@
         <f t="shared" ref="E53:G53" si="45">IF(ISNUMBER(E43), E43, "")</f>
         <v>1</v>
       </c>
-      <c r="F53" t="str">
+      <c r="F53">
         <f t="shared" si="45"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G53">
         <f t="shared" si="45"/>
@@ -2648,9 +2680,9 @@
         <f t="shared" ref="E54:G54" si="46">IF(ISNUMBER(E44), E44, "")</f>
         <v>2</v>
       </c>
-      <c r="F54" t="str">
+      <c r="F54">
         <f t="shared" si="46"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G54">
         <f t="shared" si="46"/>
@@ -2690,9 +2722,9 @@
         <f t="shared" ref="E55:G55" si="47">IF(ISNUMBER(E45), E45, "")</f>
         <v>3</v>
       </c>
-      <c r="F55" t="str">
+      <c r="F55">
         <f t="shared" si="47"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G55">
         <f t="shared" si="47"/>
@@ -2732,9 +2764,9 @@
         <f t="shared" ref="E56:G56" si="48">IF(ISNUMBER(E46), E46, "")</f>
         <v>4</v>
       </c>
-      <c r="F56" t="str">
+      <c r="F56">
         <f t="shared" si="48"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G56">
         <f t="shared" si="48"/>
@@ -2774,9 +2806,9 @@
         <f t="shared" ref="E57:G57" si="49">IF(ISNUMBER(E47), E47, "")</f>
         <v>5</v>
       </c>
-      <c r="F57" t="str">
+      <c r="F57">
         <f t="shared" si="49"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G57">
         <f t="shared" si="49"/>
@@ -2816,9 +2848,9 @@
         <f t="shared" ref="E58:G58" si="50">IF(ISNUMBER(E48), E48, "")</f>
         <v>6</v>
       </c>
-      <c r="F58" t="str">
+      <c r="F58">
         <f t="shared" si="50"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G58">
         <f t="shared" si="50"/>
@@ -2858,9 +2890,9 @@
         <f t="shared" ref="E59:G59" si="51">IF(ISNUMBER(E49), E49, "")</f>
         <v>7</v>
       </c>
-      <c r="F59" t="str">
+      <c r="F59">
         <f t="shared" si="51"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G59">
         <f t="shared" si="51"/>
@@ -2900,9 +2932,9 @@
         <f t="shared" ref="E60:G60" si="52">IF(ISNUMBER(E50), E50, "")</f>
         <v>8</v>
       </c>
-      <c r="F60" t="str">
+      <c r="F60">
         <f t="shared" si="52"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G60">
         <f t="shared" si="52"/>
@@ -2942,9 +2974,9 @@
         <f t="shared" ref="E61:G61" si="53">IF(ISNUMBER(E51), E51, "")</f>
         <v>9</v>
       </c>
-      <c r="F61" t="str">
+      <c r="F61">
         <f t="shared" si="53"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G61">
         <f t="shared" si="53"/>
@@ -3026,9 +3058,9 @@
         <f t="shared" ref="E63:G63" si="55">IF(ISNUMBER(E53), E53, "")</f>
         <v>1</v>
       </c>
-      <c r="F63" t="str">
+      <c r="F63">
         <f t="shared" si="55"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G63">
         <f t="shared" si="55"/>
@@ -3068,9 +3100,9 @@
         <f t="shared" ref="E64:G64" si="56">IF(ISNUMBER(E54), E54, "")</f>
         <v>2</v>
       </c>
-      <c r="F64" t="str">
+      <c r="F64">
         <f t="shared" si="56"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G64">
         <f t="shared" si="56"/>
@@ -3110,9 +3142,9 @@
         <f t="shared" ref="E65:G65" si="57">IF(ISNUMBER(E55), E55, "")</f>
         <v>3</v>
       </c>
-      <c r="F65" t="str">
+      <c r="F65">
         <f t="shared" si="57"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G65">
         <f t="shared" si="57"/>
@@ -3152,9 +3184,9 @@
         <f t="shared" ref="E66:G66" si="58">IF(ISNUMBER(E56), E56, "")</f>
         <v>4</v>
       </c>
-      <c r="F66" t="str">
+      <c r="F66">
         <f t="shared" si="58"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G66">
         <f t="shared" si="58"/>
@@ -3194,9 +3226,9 @@
         <f t="shared" ref="E67:G67" si="59">IF(ISNUMBER(E57), E57, "")</f>
         <v>5</v>
       </c>
-      <c r="F67" t="str">
+      <c r="F67">
         <f t="shared" si="59"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G67">
         <f t="shared" si="59"/>
@@ -3236,9 +3268,9 @@
         <f t="shared" ref="E68:G68" si="60">IF(ISNUMBER(E58), E58, "")</f>
         <v>6</v>
       </c>
-      <c r="F68" t="str">
+      <c r="F68">
         <f t="shared" si="60"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G68">
         <f t="shared" si="60"/>
@@ -3278,9 +3310,9 @@
         <f t="shared" ref="E69:G69" si="61">IF(ISNUMBER(E59), E59, "")</f>
         <v>7</v>
       </c>
-      <c r="F69" t="str">
+      <c r="F69">
         <f t="shared" si="61"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G69">
         <f t="shared" si="61"/>
@@ -3320,9 +3352,9 @@
         <f t="shared" ref="E70:G70" si="62">IF(ISNUMBER(E60), E60, "")</f>
         <v>8</v>
       </c>
-      <c r="F70" t="str">
+      <c r="F70">
         <f t="shared" si="62"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G70">
         <f t="shared" si="62"/>
@@ -3362,9 +3394,9 @@
         <f t="shared" ref="E71:G71" si="63">IF(ISNUMBER(E61), E61, "")</f>
         <v>9</v>
       </c>
-      <c r="F71" t="str">
+      <c r="F71">
         <f t="shared" si="63"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G71">
         <f t="shared" si="63"/>
@@ -3446,9 +3478,9 @@
         <f t="shared" ref="E73:G73" si="65">IF(ISNUMBER(E63), E63, "")</f>
         <v>1</v>
       </c>
-      <c r="F73" t="str">
+      <c r="F73">
         <f t="shared" si="65"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G73">
         <f t="shared" si="65"/>
@@ -3488,9 +3520,9 @@
         <f t="shared" ref="E74:G74" si="66">IF(ISNUMBER(E64), E64, "")</f>
         <v>2</v>
       </c>
-      <c r="F74" t="str">
+      <c r="F74">
         <f t="shared" si="66"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G74">
         <f t="shared" si="66"/>
@@ -3530,9 +3562,9 @@
         <f t="shared" ref="E75:G75" si="67">IF(ISNUMBER(E65), E65, "")</f>
         <v>3</v>
       </c>
-      <c r="F75" t="str">
+      <c r="F75">
         <f t="shared" si="67"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G75">
         <f t="shared" si="67"/>
@@ -3572,9 +3604,9 @@
         <f t="shared" ref="E76:G76" si="68">IF(ISNUMBER(E66), E66, "")</f>
         <v>4</v>
       </c>
-      <c r="F76" t="str">
+      <c r="F76">
         <f t="shared" si="68"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G76">
         <f t="shared" si="68"/>
@@ -3614,9 +3646,9 @@
         <f t="shared" ref="E77:G77" si="71">IF(ISNUMBER(E67), E67, "")</f>
         <v>5</v>
       </c>
-      <c r="F77" t="str">
+      <c r="F77">
         <f t="shared" si="71"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G77">
         <f t="shared" si="71"/>
@@ -3656,9 +3688,9 @@
         <f t="shared" ref="E78:G78" si="73">IF(ISNUMBER(E68), E68, "")</f>
         <v>6</v>
       </c>
-      <c r="F78" t="str">
+      <c r="F78">
         <f t="shared" si="73"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G78">
         <f t="shared" si="73"/>
@@ -3698,9 +3730,9 @@
         <f t="shared" ref="E79:G79" si="76">IF(ISNUMBER(E69), E69, "")</f>
         <v>7</v>
       </c>
-      <c r="F79" t="str">
+      <c r="F79">
         <f t="shared" si="76"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G79">
         <f t="shared" si="76"/>
@@ -3740,9 +3772,9 @@
         <f t="shared" ref="E80:G80" si="77">IF(ISNUMBER(E70), E70, "")</f>
         <v>8</v>
       </c>
-      <c r="F80" t="str">
+      <c r="F80">
         <f t="shared" si="77"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G80">
         <f t="shared" si="77"/>
@@ -3782,9 +3814,9 @@
         <f t="shared" ref="E81:G81" si="78">IF(ISNUMBER(E71), E71, "")</f>
         <v>9</v>
       </c>
-      <c r="F81" t="str">
+      <c r="F81">
         <f t="shared" si="78"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G81">
         <f t="shared" si="78"/>
@@ -3866,9 +3898,9 @@
         <f t="shared" ref="E83:G83" si="80">IF(ISNUMBER(E73), E73, "")</f>
         <v>1</v>
       </c>
-      <c r="F83" t="str">
+      <c r="F83">
         <f t="shared" si="80"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G83">
         <f t="shared" si="80"/>
@@ -3908,9 +3940,9 @@
         <f t="shared" ref="E84:G84" si="81">IF(ISNUMBER(E74), E74, "")</f>
         <v>2</v>
       </c>
-      <c r="F84" t="str">
+      <c r="F84">
         <f t="shared" si="81"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G84">
         <f t="shared" si="81"/>
@@ -3950,9 +3982,9 @@
         <f t="shared" ref="E85:G85" si="82">IF(ISNUMBER(E75), E75, "")</f>
         <v>3</v>
       </c>
-      <c r="F85" t="str">
+      <c r="F85">
         <f t="shared" si="82"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G85">
         <f t="shared" si="82"/>
@@ -3992,9 +4024,9 @@
         <f t="shared" ref="E86:G86" si="83">IF(ISNUMBER(E76), E76, "")</f>
         <v>4</v>
       </c>
-      <c r="F86" t="str">
+      <c r="F86">
         <f t="shared" si="83"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G86">
         <f t="shared" si="83"/>
@@ -4034,9 +4066,9 @@
         <f t="shared" ref="E87:G87" si="84">IF(ISNUMBER(E77), E77, "")</f>
         <v>5</v>
       </c>
-      <c r="F87" t="str">
+      <c r="F87">
         <f t="shared" si="84"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G87">
         <f t="shared" si="84"/>
@@ -4076,9 +4108,9 @@
         <f t="shared" ref="E88:G88" si="85">IF(ISNUMBER(E78), E78, "")</f>
         <v>6</v>
       </c>
-      <c r="F88" t="str">
+      <c r="F88">
         <f t="shared" si="85"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G88">
         <f t="shared" si="85"/>
@@ -4118,9 +4150,9 @@
         <f t="shared" ref="E89:G89" si="86">IF(ISNUMBER(E79), E79, "")</f>
         <v>7</v>
       </c>
-      <c r="F89" t="str">
+      <c r="F89">
         <f t="shared" si="86"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G89">
         <f t="shared" si="86"/>
@@ -4160,9 +4192,9 @@
         <f t="shared" ref="E90:G90" si="87">IF(ISNUMBER(E80), E80, "")</f>
         <v>8</v>
       </c>
-      <c r="F90" t="str">
+      <c r="F90">
         <f t="shared" si="87"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G90">
         <f t="shared" si="87"/>
@@ -4202,9 +4234,9 @@
         <f t="shared" ref="E91:G91" si="88">IF(ISNUMBER(E81), E81, "")</f>
         <v>9</v>
       </c>
-      <c r="F91" t="str">
+      <c r="F91">
         <f t="shared" si="88"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G91">
         <f t="shared" si="88"/>
@@ -4286,9 +4318,9 @@
         <f t="shared" ref="E93:G93" si="90">IF(ISNUMBER(E83), E83, "")</f>
         <v>1</v>
       </c>
-      <c r="F93" t="str">
+      <c r="F93">
         <f t="shared" si="90"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G93">
         <f t="shared" si="90"/>
@@ -4328,9 +4360,9 @@
         <f t="shared" ref="E94:G94" si="91">IF(ISNUMBER(E84), E84, "")</f>
         <v>2</v>
       </c>
-      <c r="F94" t="str">
+      <c r="F94">
         <f t="shared" si="91"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G94">
         <f t="shared" si="91"/>
@@ -4370,9 +4402,9 @@
         <f t="shared" ref="E95:G95" si="92">IF(ISNUMBER(E85), E85, "")</f>
         <v>3</v>
       </c>
-      <c r="F95" t="str">
+      <c r="F95">
         <f t="shared" si="92"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G95">
         <f t="shared" si="92"/>
@@ -4412,9 +4444,9 @@
         <f t="shared" ref="E96:G96" si="93">IF(ISNUMBER(E86), E86, "")</f>
         <v>4</v>
       </c>
-      <c r="F96" t="str">
+      <c r="F96">
         <f t="shared" si="93"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G96">
         <f t="shared" si="93"/>
@@ -4454,9 +4486,9 @@
         <f t="shared" ref="E97:G97" si="94">IF(ISNUMBER(E87), E87, "")</f>
         <v>5</v>
       </c>
-      <c r="F97" t="str">
+      <c r="F97">
         <f t="shared" si="94"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G97">
         <f t="shared" si="94"/>
@@ -4496,9 +4528,9 @@
         <f t="shared" ref="E98:G98" si="95">IF(ISNUMBER(E88), E88, "")</f>
         <v>6</v>
       </c>
-      <c r="F98" t="str">
+      <c r="F98">
         <f t="shared" si="95"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G98">
         <f t="shared" si="95"/>
@@ -4538,9 +4570,9 @@
         <f t="shared" ref="E99:G99" si="96">IF(ISNUMBER(E89), E89, "")</f>
         <v>7</v>
       </c>
-      <c r="F99" t="str">
+      <c r="F99">
         <f t="shared" si="96"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G99">
         <f t="shared" si="96"/>
@@ -4580,9 +4612,9 @@
         <f t="shared" ref="E100:G100" si="97">IF(ISNUMBER(E90), E90, "")</f>
         <v>8</v>
       </c>
-      <c r="F100" t="str">
+      <c r="F100">
         <f t="shared" si="97"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G100">
         <f t="shared" si="97"/>
@@ -4622,9 +4654,9 @@
         <f t="shared" ref="E101:G101" si="98">IF(ISNUMBER(E91), E91, "")</f>
         <v>9</v>
       </c>
-      <c r="F101" t="str">
+      <c r="F101">
         <f t="shared" si="98"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G101">
         <f t="shared" si="98"/>
@@ -4706,9 +4738,9 @@
         <f t="shared" ref="E103:G103" si="100">IF(ISNUMBER(E93), E93, "")</f>
         <v>1</v>
       </c>
-      <c r="F103" t="str">
+      <c r="F103">
         <f t="shared" si="100"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G103">
         <f t="shared" si="100"/>
@@ -4748,9 +4780,9 @@
         <f t="shared" ref="E104:G104" si="101">IF(ISNUMBER(E94), E94, "")</f>
         <v>2</v>
       </c>
-      <c r="F104" t="str">
+      <c r="F104">
         <f t="shared" si="101"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G104">
         <f t="shared" si="101"/>
@@ -4790,9 +4822,9 @@
         <f t="shared" ref="E105:G105" si="102">IF(ISNUMBER(E95), E95, "")</f>
         <v>3</v>
       </c>
-      <c r="F105" t="str">
+      <c r="F105">
         <f t="shared" si="102"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G105">
         <f t="shared" si="102"/>
@@ -4832,9 +4864,9 @@
         <f t="shared" ref="E106:G106" si="103">IF(ISNUMBER(E96), E96, "")</f>
         <v>4</v>
       </c>
-      <c r="F106" t="str">
+      <c r="F106">
         <f t="shared" si="103"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G106">
         <f t="shared" si="103"/>
@@ -4874,9 +4906,9 @@
         <f t="shared" ref="E107:G107" si="104">IF(ISNUMBER(E97), E97, "")</f>
         <v>5</v>
       </c>
-      <c r="F107" t="str">
+      <c r="F107">
         <f t="shared" si="104"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G107">
         <f t="shared" si="104"/>
@@ -4916,9 +4948,9 @@
         <f t="shared" ref="E108:G108" si="105">IF(ISNUMBER(E98), E98, "")</f>
         <v>6</v>
       </c>
-      <c r="F108" t="str">
+      <c r="F108">
         <f t="shared" si="105"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G108">
         <f t="shared" si="105"/>
@@ -4958,9 +4990,9 @@
         <f t="shared" ref="E109:G109" si="106">IF(ISNUMBER(E99), E99, "")</f>
         <v>7</v>
       </c>
-      <c r="F109" t="str">
+      <c r="F109">
         <f t="shared" si="106"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G109">
         <f t="shared" si="106"/>
@@ -5000,9 +5032,9 @@
         <f t="shared" ref="E110:G110" si="107">IF(ISNUMBER(E100), E100, "")</f>
         <v>8</v>
       </c>
-      <c r="F110" t="str">
+      <c r="F110">
         <f t="shared" si="107"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G110">
         <f t="shared" si="107"/>
@@ -5042,9 +5074,9 @@
         <f t="shared" ref="E111:G111" si="108">IF(ISNUMBER(E101), E101, "")</f>
         <v>9</v>
       </c>
-      <c r="F111" t="str">
+      <c r="F111">
         <f t="shared" si="108"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G111">
         <f t="shared" si="108"/>
@@ -5126,9 +5158,9 @@
         <f t="shared" ref="E113:G113" si="110">IF(ISNUMBER(E103), E103, "")</f>
         <v>1</v>
       </c>
-      <c r="F113" t="str">
+      <c r="F113">
         <f t="shared" si="110"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G113">
         <f t="shared" si="110"/>
@@ -5168,9 +5200,9 @@
         <f t="shared" ref="E114:G114" si="111">IF(ISNUMBER(E104), E104, "")</f>
         <v>2</v>
       </c>
-      <c r="F114" t="str">
+      <c r="F114">
         <f t="shared" si="111"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G114">
         <f t="shared" si="111"/>
@@ -5210,9 +5242,9 @@
         <f t="shared" ref="E115:G115" si="112">IF(ISNUMBER(E105), E105, "")</f>
         <v>3</v>
       </c>
-      <c r="F115" t="str">
+      <c r="F115">
         <f t="shared" si="112"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G115">
         <f t="shared" si="112"/>
@@ -5252,9 +5284,9 @@
         <f t="shared" ref="E116:G116" si="113">IF(ISNUMBER(E106), E106, "")</f>
         <v>4</v>
       </c>
-      <c r="F116" t="str">
+      <c r="F116">
         <f t="shared" si="113"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G116">
         <f t="shared" si="113"/>
@@ -5294,9 +5326,9 @@
         <f t="shared" ref="E117:G117" si="114">IF(ISNUMBER(E107), E107, "")</f>
         <v>5</v>
       </c>
-      <c r="F117" t="str">
+      <c r="F117">
         <f t="shared" si="114"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G117">
         <f t="shared" si="114"/>
@@ -5336,9 +5368,9 @@
         <f t="shared" ref="E118:G118" si="115">IF(ISNUMBER(E108), E108, "")</f>
         <v>6</v>
       </c>
-      <c r="F118" t="str">
+      <c r="F118">
         <f t="shared" si="115"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G118">
         <f t="shared" si="115"/>
@@ -5378,9 +5410,9 @@
         <f t="shared" ref="E119:G119" si="116">IF(ISNUMBER(E109), E109, "")</f>
         <v>7</v>
       </c>
-      <c r="F119" t="str">
+      <c r="F119">
         <f t="shared" si="116"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G119">
         <f t="shared" si="116"/>
@@ -5420,9 +5452,9 @@
         <f t="shared" ref="E120:G120" si="117">IF(ISNUMBER(E110), E110, "")</f>
         <v>8</v>
       </c>
-      <c r="F120" t="str">
+      <c r="F120">
         <f t="shared" si="117"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G120">
         <f t="shared" si="117"/>
@@ -5462,9 +5494,9 @@
         <f t="shared" ref="E121:G121" si="118">IF(ISNUMBER(E111), E111, "")</f>
         <v>9</v>
       </c>
-      <c r="F121" t="str">
+      <c r="F121">
         <f t="shared" si="118"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G121">
         <f t="shared" si="118"/>
@@ -5546,9 +5578,9 @@
         <f t="shared" ref="E123:G123" si="120">IF(ISNUMBER(E113), E113, "")</f>
         <v>1</v>
       </c>
-      <c r="F123" t="str">
+      <c r="F123">
         <f t="shared" si="120"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G123">
         <f t="shared" si="120"/>
@@ -5588,9 +5620,9 @@
         <f t="shared" ref="E124:G124" si="121">IF(ISNUMBER(E114), E114, "")</f>
         <v>2</v>
       </c>
-      <c r="F124" t="str">
+      <c r="F124">
         <f t="shared" si="121"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G124">
         <f t="shared" si="121"/>
@@ -5630,9 +5662,9 @@
         <f t="shared" ref="E125:G125" si="122">IF(ISNUMBER(E115), E115, "")</f>
         <v>3</v>
       </c>
-      <c r="F125" t="str">
+      <c r="F125">
         <f t="shared" si="122"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G125">
         <f t="shared" si="122"/>
@@ -5672,9 +5704,9 @@
         <f t="shared" ref="E126:G126" si="123">IF(ISNUMBER(E116), E116, "")</f>
         <v>4</v>
       </c>
-      <c r="F126" t="str">
+      <c r="F126">
         <f t="shared" si="123"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G126">
         <f t="shared" si="123"/>
@@ -5714,9 +5746,9 @@
         <f t="shared" ref="E127:G127" si="124">IF(ISNUMBER(E117), E117, "")</f>
         <v>5</v>
       </c>
-      <c r="F127" t="str">
+      <c r="F127">
         <f t="shared" si="124"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G127">
         <f t="shared" si="124"/>
@@ -5756,9 +5788,9 @@
         <f t="shared" ref="E128:G128" si="125">IF(ISNUMBER(E118), E118, "")</f>
         <v>6</v>
       </c>
-      <c r="F128" t="str">
+      <c r="F128">
         <f t="shared" si="125"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G128">
         <f t="shared" si="125"/>
@@ -5798,9 +5830,9 @@
         <f t="shared" ref="E129:G129" si="126">IF(ISNUMBER(E119), E119, "")</f>
         <v>7</v>
       </c>
-      <c r="F129" t="str">
+      <c r="F129">
         <f t="shared" si="126"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G129">
         <f t="shared" si="126"/>
@@ -5840,9 +5872,9 @@
         <f t="shared" ref="E130:G130" si="127">IF(ISNUMBER(E120), E120, "")</f>
         <v>8</v>
       </c>
-      <c r="F130" t="str">
+      <c r="F130">
         <f t="shared" si="127"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G130">
         <f t="shared" si="127"/>
@@ -5882,9 +5914,9 @@
         <f t="shared" ref="E131:G131" si="128">IF(ISNUMBER(E121), E121, "")</f>
         <v>9</v>
       </c>
-      <c r="F131" t="str">
+      <c r="F131">
         <f t="shared" si="128"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G131">
         <f t="shared" si="128"/>
@@ -5966,9 +5998,9 @@
         <f t="shared" ref="E133:G133" si="130">IF(ISNUMBER(E123), E123, "")</f>
         <v>1</v>
       </c>
-      <c r="F133" t="str">
+      <c r="F133">
         <f t="shared" si="130"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G133">
         <f t="shared" si="130"/>
@@ -6008,9 +6040,9 @@
         <f t="shared" ref="E134:G134" si="131">IF(ISNUMBER(E124), E124, "")</f>
         <v>2</v>
       </c>
-      <c r="F134" t="str">
+      <c r="F134">
         <f t="shared" si="131"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G134">
         <f t="shared" si="131"/>
@@ -6050,9 +6082,9 @@
         <f t="shared" ref="E135:G135" si="132">IF(ISNUMBER(E125), E125, "")</f>
         <v>3</v>
       </c>
-      <c r="F135" t="str">
+      <c r="F135">
         <f t="shared" si="132"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G135">
         <f t="shared" si="132"/>
@@ -6092,9 +6124,9 @@
         <f t="shared" ref="E136:G136" si="133">IF(ISNUMBER(E126), E126, "")</f>
         <v>4</v>
       </c>
-      <c r="F136" t="str">
+      <c r="F136">
         <f t="shared" si="133"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G136">
         <f t="shared" si="133"/>
@@ -6134,9 +6166,9 @@
         <f t="shared" ref="E137:G137" si="134">IF(ISNUMBER(E127), E127, "")</f>
         <v>5</v>
       </c>
-      <c r="F137" t="str">
+      <c r="F137">
         <f t="shared" si="134"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G137">
         <f t="shared" si="134"/>
@@ -6176,9 +6208,9 @@
         <f t="shared" ref="E138:G138" si="135">IF(ISNUMBER(E128), E128, "")</f>
         <v>6</v>
       </c>
-      <c r="F138" t="str">
+      <c r="F138">
         <f t="shared" si="135"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G138">
         <f t="shared" si="135"/>
@@ -6218,9 +6250,9 @@
         <f t="shared" ref="E139:G139" si="136">IF(ISNUMBER(E129), E129, "")</f>
         <v>7</v>
       </c>
-      <c r="F139" t="str">
+      <c r="F139">
         <f t="shared" si="136"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G139">
         <f t="shared" si="136"/>
@@ -6260,9 +6292,9 @@
         <f t="shared" ref="E140:G140" si="137">IF(ISNUMBER(E130), E130, "")</f>
         <v>8</v>
       </c>
-      <c r="F140" t="str">
+      <c r="F140">
         <f t="shared" si="137"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G140">
         <f t="shared" si="137"/>
@@ -6302,9 +6334,9 @@
         <f t="shared" ref="E141:G141" si="140">IF(ISNUMBER(E131), E131, "")</f>
         <v>9</v>
       </c>
-      <c r="F141" t="str">
+      <c r="F141">
         <f t="shared" si="140"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G141">
         <f t="shared" si="140"/>
@@ -6386,9 +6418,9 @@
         <f t="shared" ref="E143:G143" si="145">IF(ISNUMBER(E133), E133, "")</f>
         <v>1</v>
       </c>
-      <c r="F143" t="str">
+      <c r="F143">
         <f t="shared" si="145"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G143">
         <f t="shared" si="145"/>
@@ -6428,9 +6460,9 @@
         <f t="shared" ref="E144:G144" si="146">IF(ISNUMBER(E134), E134, "")</f>
         <v>2</v>
       </c>
-      <c r="F144" t="str">
+      <c r="F144">
         <f t="shared" si="146"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G144">
         <f t="shared" si="146"/>
@@ -6470,9 +6502,9 @@
         <f t="shared" ref="E145:G145" si="147">IF(ISNUMBER(E135), E135, "")</f>
         <v>3</v>
       </c>
-      <c r="F145" t="str">
+      <c r="F145">
         <f t="shared" si="147"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G145">
         <f t="shared" si="147"/>
@@ -6512,9 +6544,9 @@
         <f t="shared" ref="E146:G146" si="148">IF(ISNUMBER(E136), E136, "")</f>
         <v>4</v>
       </c>
-      <c r="F146" t="str">
+      <c r="F146">
         <f t="shared" si="148"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G146">
         <f t="shared" si="148"/>
@@ -6554,9 +6586,9 @@
         <f t="shared" ref="E147:G147" si="149">IF(ISNUMBER(E137), E137, "")</f>
         <v>5</v>
       </c>
-      <c r="F147" t="str">
+      <c r="F147">
         <f t="shared" si="149"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G147">
         <f t="shared" si="149"/>
@@ -6596,9 +6628,9 @@
         <f t="shared" ref="E148:G148" si="150">IF(ISNUMBER(E138), E138, "")</f>
         <v>6</v>
       </c>
-      <c r="F148" t="str">
+      <c r="F148">
         <f t="shared" si="150"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G148">
         <f t="shared" si="150"/>
@@ -6638,9 +6670,9 @@
         <f t="shared" ref="E149:G149" si="151">IF(ISNUMBER(E139), E139, "")</f>
         <v>7</v>
       </c>
-      <c r="F149" t="str">
+      <c r="F149">
         <f t="shared" si="151"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G149">
         <f t="shared" si="151"/>
@@ -6680,9 +6712,9 @@
         <f t="shared" ref="E150:G150" si="152">IF(ISNUMBER(E140), E140, "")</f>
         <v>8</v>
       </c>
-      <c r="F150" t="str">
+      <c r="F150">
         <f t="shared" si="152"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G150">
         <f t="shared" si="152"/>
@@ -6722,9 +6754,9 @@
         <f t="shared" ref="E151:G151" si="153">IF(ISNUMBER(E141), E141, "")</f>
         <v>9</v>
       </c>
-      <c r="F151" t="str">
+      <c r="F151">
         <f t="shared" si="153"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G151">
         <f t="shared" si="153"/>
@@ -6806,9 +6838,9 @@
         <f t="shared" ref="E153:G153" si="155">IF(ISNUMBER(E143), E143, "")</f>
         <v>1</v>
       </c>
-      <c r="F153" t="str">
+      <c r="F153">
         <f t="shared" si="155"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G153">
         <f t="shared" si="155"/>
@@ -6848,9 +6880,9 @@
         <f t="shared" ref="E154:G154" si="156">IF(ISNUMBER(E144), E144, "")</f>
         <v>2</v>
       </c>
-      <c r="F154" t="str">
+      <c r="F154">
         <f t="shared" si="156"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G154">
         <f t="shared" si="156"/>
@@ -6890,9 +6922,9 @@
         <f t="shared" ref="E155:G155" si="157">IF(ISNUMBER(E145), E145, "")</f>
         <v>3</v>
       </c>
-      <c r="F155" t="str">
+      <c r="F155">
         <f t="shared" si="157"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G155">
         <f t="shared" si="157"/>
@@ -6932,9 +6964,9 @@
         <f t="shared" ref="E156:G156" si="158">IF(ISNUMBER(E146), E146, "")</f>
         <v>4</v>
       </c>
-      <c r="F156" t="str">
+      <c r="F156">
         <f t="shared" si="158"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G156">
         <f t="shared" si="158"/>
@@ -6974,9 +7006,9 @@
         <f t="shared" ref="E157:G157" si="159">IF(ISNUMBER(E147), E147, "")</f>
         <v>5</v>
       </c>
-      <c r="F157" t="str">
+      <c r="F157">
         <f t="shared" si="159"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G157">
         <f t="shared" si="159"/>
@@ -7016,9 +7048,9 @@
         <f t="shared" ref="E158:G158" si="160">IF(ISNUMBER(E148), E148, "")</f>
         <v>6</v>
       </c>
-      <c r="F158" t="str">
+      <c r="F158">
         <f t="shared" si="160"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G158">
         <f t="shared" si="160"/>
@@ -7058,9 +7090,9 @@
         <f t="shared" ref="E159:G159" si="161">IF(ISNUMBER(E149), E149, "")</f>
         <v>7</v>
       </c>
-      <c r="F159" t="str">
+      <c r="F159">
         <f t="shared" si="161"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G159">
         <f t="shared" si="161"/>
@@ -7100,9 +7132,9 @@
         <f t="shared" ref="E160:G160" si="162">IF(ISNUMBER(E150), E150, "")</f>
         <v>8</v>
       </c>
-      <c r="F160" t="str">
+      <c r="F160">
         <f t="shared" si="162"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G160">
         <f t="shared" si="162"/>
@@ -7142,9 +7174,9 @@
         <f t="shared" ref="E161:G161" si="163">IF(ISNUMBER(E151), E151, "")</f>
         <v>9</v>
       </c>
-      <c r="F161" t="str">
+      <c r="F161">
         <f t="shared" si="163"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G161">
         <f t="shared" si="163"/>
@@ -7226,9 +7258,9 @@
         <f t="shared" ref="E163:G163" si="165">IF(ISNUMBER(E153), E153, "")</f>
         <v>1</v>
       </c>
-      <c r="F163" t="str">
+      <c r="F163">
         <f t="shared" si="165"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G163">
         <f t="shared" si="165"/>
@@ -7268,9 +7300,9 @@
         <f t="shared" ref="E164:G164" si="166">IF(ISNUMBER(E154), E154, "")</f>
         <v>2</v>
       </c>
-      <c r="F164" t="str">
+      <c r="F164">
         <f t="shared" si="166"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G164">
         <f t="shared" si="166"/>
@@ -7310,9 +7342,9 @@
         <f t="shared" ref="E165:G165" si="167">IF(ISNUMBER(E155), E155, "")</f>
         <v>3</v>
       </c>
-      <c r="F165" t="str">
+      <c r="F165">
         <f t="shared" si="167"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G165">
         <f t="shared" si="167"/>
@@ -7352,9 +7384,9 @@
         <f t="shared" ref="E166:G166" si="168">IF(ISNUMBER(E156), E156, "")</f>
         <v>4</v>
       </c>
-      <c r="F166" t="str">
+      <c r="F166">
         <f t="shared" si="168"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G166">
         <f t="shared" si="168"/>
@@ -7394,9 +7426,9 @@
         <f t="shared" ref="E167:G167" si="169">IF(ISNUMBER(E157), E157, "")</f>
         <v>5</v>
       </c>
-      <c r="F167" t="str">
+      <c r="F167">
         <f t="shared" si="169"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G167">
         <f t="shared" si="169"/>
@@ -7436,9 +7468,9 @@
         <f t="shared" ref="E168:G168" si="170">IF(ISNUMBER(E158), E158, "")</f>
         <v>6</v>
       </c>
-      <c r="F168" t="str">
+      <c r="F168">
         <f t="shared" si="170"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G168">
         <f t="shared" si="170"/>
@@ -7478,9 +7510,9 @@
         <f t="shared" ref="E169:G169" si="171">IF(ISNUMBER(E159), E159, "")</f>
         <v>7</v>
       </c>
-      <c r="F169" t="str">
+      <c r="F169">
         <f t="shared" si="171"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G169">
         <f t="shared" si="171"/>
@@ -7520,9 +7552,9 @@
         <f t="shared" ref="E170:G170" si="172">IF(ISNUMBER(E160), E160, "")</f>
         <v>8</v>
       </c>
-      <c r="F170" t="str">
+      <c r="F170">
         <f t="shared" si="172"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G170">
         <f t="shared" si="172"/>
@@ -7562,9 +7594,9 @@
         <f t="shared" ref="E171:G171" si="173">IF(ISNUMBER(E161), E161, "")</f>
         <v>9</v>
       </c>
-      <c r="F171" t="str">
+      <c r="F171">
         <f t="shared" si="173"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G171">
         <f t="shared" si="173"/>
@@ -7646,9 +7678,9 @@
         <f t="shared" ref="E173:G173" si="175">IF(ISNUMBER(E163), E163, "")</f>
         <v>1</v>
       </c>
-      <c r="F173" t="str">
+      <c r="F173">
         <f t="shared" si="175"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G173">
         <f t="shared" si="175"/>
@@ -7688,9 +7720,9 @@
         <f t="shared" ref="E174:G174" si="176">IF(ISNUMBER(E164), E164, "")</f>
         <v>2</v>
       </c>
-      <c r="F174" t="str">
+      <c r="F174">
         <f t="shared" si="176"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G174">
         <f t="shared" si="176"/>
@@ -7730,9 +7762,9 @@
         <f t="shared" ref="E175:G175" si="177">IF(ISNUMBER(E165), E165, "")</f>
         <v>3</v>
       </c>
-      <c r="F175" t="str">
+      <c r="F175">
         <f t="shared" si="177"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G175">
         <f t="shared" si="177"/>
@@ -7772,9 +7804,9 @@
         <f t="shared" ref="E176:G176" si="178">IF(ISNUMBER(E166), E166, "")</f>
         <v>4</v>
       </c>
-      <c r="F176" t="str">
+      <c r="F176">
         <f t="shared" si="178"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G176">
         <f t="shared" si="178"/>
@@ -7814,9 +7846,9 @@
         <f t="shared" ref="E177:G177" si="179">IF(ISNUMBER(E167), E167, "")</f>
         <v>5</v>
       </c>
-      <c r="F177" t="str">
+      <c r="F177">
         <f t="shared" si="179"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G177">
         <f t="shared" si="179"/>
@@ -7856,9 +7888,9 @@
         <f t="shared" ref="E178:G178" si="180">IF(ISNUMBER(E168), E168, "")</f>
         <v>6</v>
       </c>
-      <c r="F178" t="str">
+      <c r="F178">
         <f t="shared" si="180"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G178">
         <f t="shared" si="180"/>
@@ -7898,9 +7930,9 @@
         <f t="shared" ref="E179:G179" si="181">IF(ISNUMBER(E169), E169, "")</f>
         <v>7</v>
       </c>
-      <c r="F179" t="str">
+      <c r="F179">
         <f t="shared" si="181"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G179">
         <f t="shared" si="181"/>
@@ -7940,9 +7972,9 @@
         <f t="shared" ref="E180:G180" si="182">IF(ISNUMBER(E170), E170, "")</f>
         <v>8</v>
       </c>
-      <c r="F180" t="str">
+      <c r="F180">
         <f t="shared" si="182"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G180">
         <f t="shared" si="182"/>
@@ -7982,9 +8014,9 @@
         <f t="shared" ref="E181:G181" si="183">IF(ISNUMBER(E171), E171, "")</f>
         <v>9</v>
       </c>
-      <c r="F181" t="str">
+      <c r="F181">
         <f t="shared" si="183"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G181">
         <f t="shared" si="183"/>
@@ -8066,9 +8098,9 @@
         <f t="shared" ref="E183:G183" si="185">IF(ISNUMBER(E173), E173, "")</f>
         <v>1</v>
       </c>
-      <c r="F183" t="str">
+      <c r="F183">
         <f t="shared" si="185"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G183">
         <f t="shared" si="185"/>
@@ -8108,9 +8140,9 @@
         <f t="shared" ref="E184:G184" si="186">IF(ISNUMBER(E174), E174, "")</f>
         <v>2</v>
       </c>
-      <c r="F184" t="str">
+      <c r="F184">
         <f t="shared" si="186"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G184">
         <f t="shared" si="186"/>
@@ -8150,9 +8182,9 @@
         <f t="shared" ref="E185:G185" si="187">IF(ISNUMBER(E175), E175, "")</f>
         <v>3</v>
       </c>
-      <c r="F185" t="str">
+      <c r="F185">
         <f t="shared" si="187"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G185">
         <f t="shared" si="187"/>
@@ -8192,9 +8224,9 @@
         <f t="shared" ref="E186:G186" si="188">IF(ISNUMBER(E176), E176, "")</f>
         <v>4</v>
       </c>
-      <c r="F186" t="str">
+      <c r="F186">
         <f t="shared" si="188"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G186">
         <f t="shared" si="188"/>
@@ -8234,9 +8266,9 @@
         <f t="shared" ref="E187:G187" si="189">IF(ISNUMBER(E177), E177, "")</f>
         <v>5</v>
       </c>
-      <c r="F187" t="str">
+      <c r="F187">
         <f t="shared" si="189"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G187">
         <f t="shared" si="189"/>
@@ -8276,9 +8308,9 @@
         <f t="shared" ref="E188:G188" si="190">IF(ISNUMBER(E178), E178, "")</f>
         <v>6</v>
       </c>
-      <c r="F188" t="str">
+      <c r="F188">
         <f t="shared" si="190"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G188">
         <f t="shared" si="190"/>
@@ -8318,9 +8350,9 @@
         <f t="shared" ref="E189:G189" si="191">IF(ISNUMBER(E179), E179, "")</f>
         <v>7</v>
       </c>
-      <c r="F189" t="str">
+      <c r="F189">
         <f t="shared" si="191"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G189">
         <f t="shared" si="191"/>
@@ -8360,9 +8392,9 @@
         <f t="shared" ref="E190:G190" si="192">IF(ISNUMBER(E180), E180, "")</f>
         <v>8</v>
       </c>
-      <c r="F190" t="str">
+      <c r="F190">
         <f t="shared" si="192"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G190">
         <f t="shared" si="192"/>
@@ -8402,9 +8434,9 @@
         <f t="shared" ref="E191:G191" si="193">IF(ISNUMBER(E181), E181, "")</f>
         <v>9</v>
       </c>
-      <c r="F191" t="str">
+      <c r="F191">
         <f t="shared" si="193"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G191">
         <f t="shared" si="193"/>
@@ -8486,9 +8518,9 @@
         <f t="shared" ref="E193:G193" si="195">IF(ISNUMBER(E183), E183, "")</f>
         <v>1</v>
       </c>
-      <c r="F193" t="str">
+      <c r="F193">
         <f t="shared" si="195"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G193">
         <f t="shared" si="195"/>
@@ -8528,9 +8560,9 @@
         <f t="shared" ref="E194:G194" si="196">IF(ISNUMBER(E184), E184, "")</f>
         <v>2</v>
       </c>
-      <c r="F194" t="str">
+      <c r="F194">
         <f t="shared" si="196"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G194">
         <f t="shared" si="196"/>
@@ -8570,9 +8602,9 @@
         <f t="shared" ref="E195:G195" si="197">IF(ISNUMBER(E185), E185, "")</f>
         <v>3</v>
       </c>
-      <c r="F195" t="str">
+      <c r="F195">
         <f t="shared" si="197"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G195">
         <f t="shared" si="197"/>
@@ -8612,9 +8644,9 @@
         <f t="shared" ref="E196:G196" si="198">IF(ISNUMBER(E186), E186, "")</f>
         <v>4</v>
       </c>
-      <c r="F196" t="str">
+      <c r="F196">
         <f t="shared" si="198"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G196">
         <f t="shared" si="198"/>
@@ -8654,9 +8686,9 @@
         <f t="shared" ref="E197:G197" si="199">IF(ISNUMBER(E187), E187, "")</f>
         <v>5</v>
       </c>
-      <c r="F197" t="str">
+      <c r="F197">
         <f t="shared" si="199"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G197">
         <f t="shared" si="199"/>
@@ -8696,9 +8728,9 @@
         <f t="shared" ref="E198:G198" si="200">IF(ISNUMBER(E188), E188, "")</f>
         <v>6</v>
       </c>
-      <c r="F198" t="str">
+      <c r="F198">
         <f t="shared" si="200"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G198">
         <f t="shared" si="200"/>
@@ -8738,9 +8770,9 @@
         <f t="shared" ref="E199:G199" si="201">IF(ISNUMBER(E189), E189, "")</f>
         <v>7</v>
       </c>
-      <c r="F199" t="str">
+      <c r="F199">
         <f t="shared" si="201"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G199">
         <f t="shared" si="201"/>
@@ -8780,9 +8812,9 @@
         <f t="shared" ref="E200:G200" si="202">IF(ISNUMBER(E190), E190, "")</f>
         <v>8</v>
       </c>
-      <c r="F200" t="str">
+      <c r="F200">
         <f t="shared" si="202"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G200">
         <f t="shared" si="202"/>
@@ -8822,9 +8854,9 @@
         <f t="shared" ref="E201:G201" si="203">IF(ISNUMBER(E191), E191, "")</f>
         <v>9</v>
       </c>
-      <c r="F201" t="str">
+      <c r="F201">
         <f t="shared" si="203"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G201">
         <f t="shared" si="203"/>
@@ -8906,9 +8938,9 @@
         <f t="shared" ref="E203:G203" si="205">IF(ISNUMBER(E193), E193, "")</f>
         <v>1</v>
       </c>
-      <c r="F203" t="str">
+      <c r="F203">
         <f t="shared" si="205"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G203">
         <f t="shared" si="205"/>
@@ -8951,9 +8983,9 @@
         <f t="shared" ref="E204:G204" si="206">IF(ISNUMBER(E194), E194, "")</f>
         <v>2</v>
       </c>
-      <c r="F204" t="str">
+      <c r="F204">
         <f t="shared" si="206"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G204">
         <f t="shared" si="206"/>
@@ -8993,9 +9025,9 @@
         <f t="shared" ref="E205:G205" si="209">IF(ISNUMBER(E195), E195, "")</f>
         <v>3</v>
       </c>
-      <c r="F205" t="str">
+      <c r="F205">
         <f t="shared" si="209"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G205">
         <f t="shared" si="209"/>
@@ -9035,9 +9067,9 @@
         <f t="shared" ref="E206:G206" si="211">IF(ISNUMBER(E196), E196, "")</f>
         <v>4</v>
       </c>
-      <c r="F206" t="str">
+      <c r="F206">
         <f t="shared" si="211"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G206">
         <f t="shared" si="211"/>
@@ -9077,9 +9109,9 @@
         <f t="shared" ref="E207:G207" si="214">IF(ISNUMBER(E197), E197, "")</f>
         <v>5</v>
       </c>
-      <c r="F207" t="str">
+      <c r="F207">
         <f t="shared" si="214"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G207">
         <f t="shared" si="214"/>
@@ -9119,9 +9151,9 @@
         <f t="shared" ref="E208:G208" si="215">IF(ISNUMBER(E198), E198, "")</f>
         <v>6</v>
       </c>
-      <c r="F208" t="str">
+      <c r="F208">
         <f t="shared" si="215"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G208">
         <f t="shared" si="215"/>
@@ -9161,9 +9193,9 @@
         <f t="shared" ref="E209:G209" si="216">IF(ISNUMBER(E199), E199, "")</f>
         <v>7</v>
       </c>
-      <c r="F209" t="str">
+      <c r="F209">
         <f t="shared" si="216"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G209">
         <f t="shared" si="216"/>
@@ -9203,9 +9235,9 @@
         <f t="shared" ref="E210:G210" si="217">IF(ISNUMBER(E200), E200, "")</f>
         <v>8</v>
       </c>
-      <c r="F210" t="str">
+      <c r="F210">
         <f t="shared" si="217"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G210">
         <f t="shared" si="217"/>
@@ -9245,9 +9277,9 @@
         <f t="shared" ref="E211:G211" si="218">IF(ISNUMBER(E201), E201, "")</f>
         <v>9</v>
       </c>
-      <c r="F211" t="str">
+      <c r="F211">
         <f t="shared" si="218"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G211">
         <f t="shared" si="218"/>
@@ -9329,9 +9361,9 @@
         <f t="shared" ref="E213:G213" si="220">IF(ISNUMBER(E203), E203, "")</f>
         <v>1</v>
       </c>
-      <c r="F213" t="str">
+      <c r="F213">
         <f t="shared" si="220"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G213">
         <f t="shared" si="220"/>
@@ -9371,9 +9403,9 @@
         <f t="shared" ref="E214:G214" si="221">IF(ISNUMBER(E204), E204, "")</f>
         <v>2</v>
       </c>
-      <c r="F214" t="str">
+      <c r="F214">
         <f t="shared" si="221"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G214">
         <f t="shared" si="221"/>
@@ -9413,9 +9445,9 @@
         <f t="shared" ref="E215:G215" si="222">IF(ISNUMBER(E205), E205, "")</f>
         <v>3</v>
       </c>
-      <c r="F215" t="str">
+      <c r="F215">
         <f t="shared" si="222"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G215">
         <f t="shared" si="222"/>
@@ -9455,9 +9487,9 @@
         <f t="shared" ref="E216:G216" si="223">IF(ISNUMBER(E206), E206, "")</f>
         <v>4</v>
       </c>
-      <c r="F216" t="str">
+      <c r="F216">
         <f t="shared" si="223"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G216">
         <f t="shared" si="223"/>
@@ -9497,9 +9529,9 @@
         <f t="shared" ref="E217:G217" si="224">IF(ISNUMBER(E207), E207, "")</f>
         <v>5</v>
       </c>
-      <c r="F217" t="str">
+      <c r="F217">
         <f t="shared" si="224"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G217">
         <f t="shared" si="224"/>
@@ -9539,9 +9571,9 @@
         <f t="shared" ref="E218:G218" si="225">IF(ISNUMBER(E208), E208, "")</f>
         <v>6</v>
       </c>
-      <c r="F218" t="str">
+      <c r="F218">
         <f t="shared" si="225"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G218">
         <f t="shared" si="225"/>
@@ -9581,9 +9613,9 @@
         <f t="shared" ref="E219:G219" si="226">IF(ISNUMBER(E209), E209, "")</f>
         <v>7</v>
       </c>
-      <c r="F219" t="str">
+      <c r="F219">
         <f t="shared" si="226"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G219">
         <f t="shared" si="226"/>
@@ -9623,9 +9655,9 @@
         <f t="shared" ref="E220:G220" si="227">IF(ISNUMBER(E210), E210, "")</f>
         <v>8</v>
       </c>
-      <c r="F220" t="str">
+      <c r="F220">
         <f t="shared" si="227"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G220">
         <f t="shared" si="227"/>
@@ -9665,9 +9697,9 @@
         <f t="shared" ref="E221:G221" si="228">IF(ISNUMBER(E211), E211, "")</f>
         <v>9</v>
       </c>
-      <c r="F221" t="str">
+      <c r="F221">
         <f t="shared" si="228"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G221">
         <f t="shared" si="228"/>
@@ -9749,9 +9781,9 @@
         <f t="shared" ref="E223:G223" si="230">IF(ISNUMBER(E213), E213, "")</f>
         <v>1</v>
       </c>
-      <c r="F223" t="str">
+      <c r="F223">
         <f t="shared" si="230"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G223">
         <f t="shared" si="230"/>
@@ -9791,9 +9823,9 @@
         <f t="shared" ref="E224:G224" si="231">IF(ISNUMBER(E214), E214, "")</f>
         <v>2</v>
       </c>
-      <c r="F224" t="str">
+      <c r="F224">
         <f t="shared" si="231"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G224">
         <f t="shared" si="231"/>
@@ -9833,9 +9865,9 @@
         <f t="shared" ref="E225:G225" si="232">IF(ISNUMBER(E215), E215, "")</f>
         <v>3</v>
       </c>
-      <c r="F225" t="str">
+      <c r="F225">
         <f t="shared" si="232"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G225">
         <f t="shared" si="232"/>
@@ -9875,9 +9907,9 @@
         <f t="shared" ref="E226:G226" si="233">IF(ISNUMBER(E216), E216, "")</f>
         <v>4</v>
       </c>
-      <c r="F226" t="str">
+      <c r="F226">
         <f t="shared" si="233"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G226">
         <f t="shared" si="233"/>
@@ -9917,9 +9949,9 @@
         <f t="shared" ref="E227:G227" si="234">IF(ISNUMBER(E217), E217, "")</f>
         <v>5</v>
       </c>
-      <c r="F227" t="str">
+      <c r="F227">
         <f t="shared" si="234"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G227">
         <f t="shared" si="234"/>
@@ -9959,9 +9991,9 @@
         <f t="shared" ref="E228:G228" si="235">IF(ISNUMBER(E218), E218, "")</f>
         <v>6</v>
       </c>
-      <c r="F228" t="str">
+      <c r="F228">
         <f t="shared" si="235"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G228">
         <f t="shared" si="235"/>
@@ -10001,9 +10033,9 @@
         <f t="shared" ref="E229:G229" si="236">IF(ISNUMBER(E219), E219, "")</f>
         <v>7</v>
       </c>
-      <c r="F229" t="str">
+      <c r="F229">
         <f t="shared" si="236"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G229">
         <f t="shared" si="236"/>
@@ -10043,9 +10075,9 @@
         <f t="shared" ref="E230:G230" si="237">IF(ISNUMBER(E220), E220, "")</f>
         <v>8</v>
       </c>
-      <c r="F230" t="str">
+      <c r="F230">
         <f t="shared" si="237"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G230">
         <f t="shared" si="237"/>
@@ -10085,9 +10117,9 @@
         <f t="shared" ref="E231:G231" si="238">IF(ISNUMBER(E221), E221, "")</f>
         <v>9</v>
       </c>
-      <c r="F231" t="str">
+      <c r="F231">
         <f t="shared" si="238"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G231">
         <f t="shared" si="238"/>
@@ -10169,9 +10201,9 @@
         <f t="shared" ref="E233:G233" si="240">IF(ISNUMBER(E223), E223, "")</f>
         <v>1</v>
       </c>
-      <c r="F233" t="str">
+      <c r="F233">
         <f t="shared" si="240"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G233">
         <f t="shared" si="240"/>
@@ -10211,9 +10243,9 @@
         <f t="shared" ref="E234:G234" si="241">IF(ISNUMBER(E224), E224, "")</f>
         <v>2</v>
       </c>
-      <c r="F234" t="str">
+      <c r="F234">
         <f t="shared" si="241"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G234">
         <f t="shared" si="241"/>
@@ -10253,9 +10285,9 @@
         <f t="shared" ref="E235:G235" si="242">IF(ISNUMBER(E225), E225, "")</f>
         <v>3</v>
       </c>
-      <c r="F235" t="str">
+      <c r="F235">
         <f t="shared" si="242"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G235">
         <f t="shared" si="242"/>
@@ -10295,9 +10327,9 @@
         <f t="shared" ref="E236:G236" si="243">IF(ISNUMBER(E226), E226, "")</f>
         <v>4</v>
       </c>
-      <c r="F236" t="str">
+      <c r="F236">
         <f t="shared" si="243"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G236">
         <f t="shared" si="243"/>
@@ -10337,9 +10369,9 @@
         <f t="shared" ref="E237:G237" si="244">IF(ISNUMBER(E227), E227, "")</f>
         <v>5</v>
       </c>
-      <c r="F237" t="str">
+      <c r="F237">
         <f t="shared" si="244"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G237">
         <f t="shared" si="244"/>
@@ -10379,9 +10411,9 @@
         <f t="shared" ref="E238:G238" si="245">IF(ISNUMBER(E228), E228, "")</f>
         <v>6</v>
       </c>
-      <c r="F238" t="str">
+      <c r="F238">
         <f t="shared" si="245"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G238">
         <f t="shared" si="245"/>
@@ -10421,9 +10453,9 @@
         <f t="shared" ref="E239:G239" si="246">IF(ISNUMBER(E229), E229, "")</f>
         <v>7</v>
       </c>
-      <c r="F239" t="str">
+      <c r="F239">
         <f t="shared" si="246"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G239">
         <f t="shared" si="246"/>
@@ -10463,9 +10495,9 @@
         <f t="shared" ref="E240:G240" si="247">IF(ISNUMBER(E230), E230, "")</f>
         <v>8</v>
       </c>
-      <c r="F240" t="str">
+      <c r="F240">
         <f t="shared" si="247"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G240">
         <f t="shared" si="247"/>
@@ -10505,9 +10537,9 @@
         <f t="shared" ref="E241:G241" si="248">IF(ISNUMBER(E231), E231, "")</f>
         <v>9</v>
       </c>
-      <c r="F241" t="str">
+      <c r="F241">
         <f t="shared" si="248"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G241">
         <f t="shared" si="248"/>
@@ -10589,9 +10621,9 @@
         <f t="shared" ref="E243:G243" si="250">IF(ISNUMBER(E233), E233, "")</f>
         <v>1</v>
       </c>
-      <c r="F243" t="str">
+      <c r="F243">
         <f t="shared" si="250"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G243">
         <f t="shared" si="250"/>
@@ -10631,9 +10663,9 @@
         <f t="shared" ref="E244:G244" si="251">IF(ISNUMBER(E234), E234, "")</f>
         <v>2</v>
       </c>
-      <c r="F244" t="str">
+      <c r="F244">
         <f t="shared" si="251"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G244">
         <f t="shared" si="251"/>
@@ -10673,9 +10705,9 @@
         <f t="shared" ref="E245:G245" si="252">IF(ISNUMBER(E235), E235, "")</f>
         <v>3</v>
       </c>
-      <c r="F245" t="str">
+      <c r="F245">
         <f t="shared" si="252"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G245">
         <f t="shared" si="252"/>
@@ -10715,9 +10747,9 @@
         <f t="shared" ref="E246:G246" si="253">IF(ISNUMBER(E236), E236, "")</f>
         <v>4</v>
       </c>
-      <c r="F246" t="str">
+      <c r="F246">
         <f t="shared" si="253"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G246">
         <f t="shared" si="253"/>
@@ -10757,9 +10789,9 @@
         <f t="shared" ref="E247:G247" si="254">IF(ISNUMBER(E237), E237, "")</f>
         <v>5</v>
       </c>
-      <c r="F247" t="str">
+      <c r="F247">
         <f t="shared" si="254"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G247">
         <f t="shared" si="254"/>
@@ -10799,9 +10831,9 @@
         <f t="shared" ref="E248:G248" si="255">IF(ISNUMBER(E238), E238, "")</f>
         <v>6</v>
       </c>
-      <c r="F248" t="str">
+      <c r="F248">
         <f t="shared" si="255"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G248">
         <f t="shared" si="255"/>
@@ -10841,9 +10873,9 @@
         <f t="shared" ref="E249:G249" si="256">IF(ISNUMBER(E239), E239, "")</f>
         <v>7</v>
       </c>
-      <c r="F249" t="str">
+      <c r="F249">
         <f t="shared" si="256"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G249">
         <f t="shared" si="256"/>
@@ -10883,9 +10915,9 @@
         <f t="shared" ref="E250:G250" si="257">IF(ISNUMBER(E240), E240, "")</f>
         <v>8</v>
       </c>
-      <c r="F250" t="str">
+      <c r="F250">
         <f t="shared" si="257"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G250">
         <f t="shared" si="257"/>
@@ -10925,9 +10957,9 @@
         <f t="shared" ref="E251:G251" si="258">IF(ISNUMBER(E241), E241, "")</f>
         <v>9</v>
       </c>
-      <c r="F251" t="str">
+      <c r="F251">
         <f t="shared" si="258"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G251">
         <f t="shared" si="258"/>
@@ -11009,9 +11041,9 @@
         <f t="shared" ref="E253:G253" si="260">IF(ISNUMBER(E243), E243, "")</f>
         <v>1</v>
       </c>
-      <c r="F253" t="str">
+      <c r="F253">
         <f t="shared" si="260"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G253">
         <f t="shared" si="260"/>
@@ -11051,9 +11083,9 @@
         <f t="shared" ref="E254:G254" si="261">IF(ISNUMBER(E244), E244, "")</f>
         <v>2</v>
       </c>
-      <c r="F254" t="str">
+      <c r="F254">
         <f t="shared" si="261"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G254">
         <f t="shared" si="261"/>
@@ -11093,9 +11125,9 @@
         <f t="shared" ref="E255:G255" si="262">IF(ISNUMBER(E245), E245, "")</f>
         <v>3</v>
       </c>
-      <c r="F255" t="str">
+      <c r="F255">
         <f t="shared" si="262"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G255">
         <f t="shared" si="262"/>
@@ -11135,9 +11167,9 @@
         <f t="shared" ref="E256:G256" si="263">IF(ISNUMBER(E246), E246, "")</f>
         <v>4</v>
       </c>
-      <c r="F256" t="str">
+      <c r="F256">
         <f t="shared" si="263"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G256">
         <f t="shared" si="263"/>
@@ -11177,9 +11209,9 @@
         <f t="shared" ref="E257:G257" si="264">IF(ISNUMBER(E247), E247, "")</f>
         <v>5</v>
       </c>
-      <c r="F257" t="str">
+      <c r="F257">
         <f t="shared" si="264"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G257">
         <f t="shared" si="264"/>
@@ -11219,9 +11251,9 @@
         <f t="shared" ref="E258:G258" si="265">IF(ISNUMBER(E248), E248, "")</f>
         <v>6</v>
       </c>
-      <c r="F258" t="str">
+      <c r="F258">
         <f t="shared" si="265"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G258">
         <f t="shared" si="265"/>
@@ -11261,9 +11293,9 @@
         <f t="shared" ref="E259:G259" si="266">IF(ISNUMBER(E249), E249, "")</f>
         <v>7</v>
       </c>
-      <c r="F259" t="str">
+      <c r="F259">
         <f t="shared" si="266"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G259">
         <f t="shared" si="266"/>
@@ -11303,9 +11335,9 @@
         <f t="shared" ref="E260:G260" si="267">IF(ISNUMBER(E250), E250, "")</f>
         <v>8</v>
       </c>
-      <c r="F260" t="str">
+      <c r="F260">
         <f t="shared" si="267"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G260">
         <f t="shared" si="267"/>
@@ -11345,9 +11377,9 @@
         <f t="shared" ref="E261:G261" si="268">IF(ISNUMBER(E251), E251, "")</f>
         <v>9</v>
       </c>
-      <c r="F261" t="str">
+      <c r="F261">
         <f t="shared" si="268"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G261">
         <f t="shared" si="268"/>
@@ -11429,9 +11461,9 @@
         <f t="shared" ref="E263:G263" si="270">IF(ISNUMBER(E253), E253, "")</f>
         <v>1</v>
       </c>
-      <c r="F263" t="str">
+      <c r="F263">
         <f t="shared" si="270"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G263">
         <f t="shared" si="270"/>
@@ -11471,9 +11503,9 @@
         <f t="shared" ref="E264:G264" si="271">IF(ISNUMBER(E254), E254, "")</f>
         <v>2</v>
       </c>
-      <c r="F264" t="str">
+      <c r="F264">
         <f t="shared" si="271"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G264">
         <f t="shared" si="271"/>
@@ -11513,9 +11545,9 @@
         <f t="shared" ref="E265:G265" si="272">IF(ISNUMBER(E255), E255, "")</f>
         <v>3</v>
       </c>
-      <c r="F265" t="str">
+      <c r="F265">
         <f t="shared" si="272"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G265">
         <f t="shared" si="272"/>
@@ -11555,9 +11587,9 @@
         <f t="shared" ref="E266:G266" si="273">IF(ISNUMBER(E256), E256, "")</f>
         <v>4</v>
       </c>
-      <c r="F266" t="str">
+      <c r="F266">
         <f t="shared" si="273"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G266">
         <f t="shared" si="273"/>
@@ -11597,9 +11629,9 @@
         <f t="shared" ref="E267:G267" si="274">IF(ISNUMBER(E257), E257, "")</f>
         <v>5</v>
       </c>
-      <c r="F267" t="str">
+      <c r="F267">
         <f t="shared" si="274"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G267">
         <f t="shared" si="274"/>
@@ -11639,9 +11671,9 @@
         <f t="shared" ref="E268:G268" si="275">IF(ISNUMBER(E258), E258, "")</f>
         <v>6</v>
       </c>
-      <c r="F268" t="str">
+      <c r="F268">
         <f t="shared" si="275"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G268">
         <f t="shared" si="275"/>
@@ -11681,9 +11713,9 @@
         <f t="shared" ref="E269:G269" si="278">IF(ISNUMBER(E259), E259, "")</f>
         <v>7</v>
       </c>
-      <c r="F269" t="str">
+      <c r="F269">
         <f t="shared" si="278"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G269">
         <f t="shared" si="278"/>
@@ -11723,9 +11755,9 @@
         <f t="shared" ref="E270:G270" si="280">IF(ISNUMBER(E260), E260, "")</f>
         <v>8</v>
       </c>
-      <c r="F270" t="str">
+      <c r="F270">
         <f t="shared" si="280"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G270">
         <f t="shared" si="280"/>
@@ -11765,9 +11797,9 @@
         <f t="shared" ref="E271:G271" si="283">IF(ISNUMBER(E261), E261, "")</f>
         <v>9</v>
       </c>
-      <c r="F271" t="str">
+      <c r="F271">
         <f t="shared" si="283"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G271">
         <f t="shared" si="283"/>
@@ -11849,9 +11881,9 @@
         <f t="shared" ref="E273:G273" si="285">IF(ISNUMBER(E263), E263, "")</f>
         <v>1</v>
       </c>
-      <c r="F273" t="str">
+      <c r="F273">
         <f t="shared" si="285"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G273">
         <f t="shared" si="285"/>
@@ -11891,9 +11923,9 @@
         <f t="shared" ref="E274:G274" si="286">IF(ISNUMBER(E264), E264, "")</f>
         <v>2</v>
       </c>
-      <c r="F274" t="str">
+      <c r="F274">
         <f t="shared" si="286"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G274">
         <f t="shared" si="286"/>
@@ -11933,9 +11965,9 @@
         <f t="shared" ref="E275:G275" si="287">IF(ISNUMBER(E265), E265, "")</f>
         <v>3</v>
       </c>
-      <c r="F275" t="str">
+      <c r="F275">
         <f t="shared" si="287"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G275">
         <f t="shared" si="287"/>
@@ -11975,9 +12007,9 @@
         <f t="shared" ref="E276:G276" si="288">IF(ISNUMBER(E266), E266, "")</f>
         <v>4</v>
       </c>
-      <c r="F276" t="str">
+      <c r="F276">
         <f t="shared" si="288"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G276">
         <f t="shared" si="288"/>
@@ -12017,9 +12049,9 @@
         <f t="shared" ref="E277:G277" si="289">IF(ISNUMBER(E267), E267, "")</f>
         <v>5</v>
       </c>
-      <c r="F277" t="str">
+      <c r="F277">
         <f t="shared" si="289"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G277">
         <f t="shared" si="289"/>
@@ -12059,9 +12091,9 @@
         <f t="shared" ref="E278:G278" si="290">IF(ISNUMBER(E268), E268, "")</f>
         <v>6</v>
       </c>
-      <c r="F278" t="str">
+      <c r="F278">
         <f t="shared" si="290"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G278">
         <f t="shared" si="290"/>
@@ -12101,9 +12133,9 @@
         <f t="shared" ref="E279:G279" si="291">IF(ISNUMBER(E269), E269, "")</f>
         <v>7</v>
       </c>
-      <c r="F279" t="str">
+      <c r="F279">
         <f t="shared" si="291"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G279">
         <f t="shared" si="291"/>
@@ -12143,9 +12175,9 @@
         <f t="shared" ref="E280:G280" si="292">IF(ISNUMBER(E270), E270, "")</f>
         <v>8</v>
       </c>
-      <c r="F280" t="str">
+      <c r="F280">
         <f t="shared" si="292"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G280">
         <f t="shared" si="292"/>
@@ -12185,9 +12217,9 @@
         <f t="shared" ref="E281:G281" si="293">IF(ISNUMBER(E271), E271, "")</f>
         <v>9</v>
       </c>
-      <c r="F281" t="str">
+      <c r="F281">
         <f t="shared" si="293"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G281">
         <f t="shared" si="293"/>
@@ -12269,9 +12301,9 @@
         <f t="shared" ref="E283:G283" si="295">IF(ISNUMBER(E273), E273, "")</f>
         <v>1</v>
       </c>
-      <c r="F283" t="str">
+      <c r="F283">
         <f t="shared" si="295"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G283">
         <f t="shared" si="295"/>
@@ -12311,9 +12343,9 @@
         <f t="shared" ref="E284:G284" si="296">IF(ISNUMBER(E274), E274, "")</f>
         <v>2</v>
       </c>
-      <c r="F284" t="str">
+      <c r="F284">
         <f t="shared" si="296"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G284">
         <f t="shared" si="296"/>
@@ -12353,9 +12385,9 @@
         <f t="shared" ref="E285:G285" si="297">IF(ISNUMBER(E275), E275, "")</f>
         <v>3</v>
       </c>
-      <c r="F285" t="str">
+      <c r="F285">
         <f t="shared" si="297"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G285">
         <f t="shared" si="297"/>
@@ -12395,9 +12427,9 @@
         <f t="shared" ref="E286:G286" si="298">IF(ISNUMBER(E276), E276, "")</f>
         <v>4</v>
       </c>
-      <c r="F286" t="str">
+      <c r="F286">
         <f t="shared" si="298"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G286">
         <f t="shared" si="298"/>
@@ -12437,9 +12469,9 @@
         <f t="shared" ref="E287:G287" si="299">IF(ISNUMBER(E277), E277, "")</f>
         <v>5</v>
       </c>
-      <c r="F287" t="str">
+      <c r="F287">
         <f t="shared" si="299"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G287">
         <f t="shared" si="299"/>
@@ -12479,9 +12511,9 @@
         <f t="shared" ref="E288:G288" si="300">IF(ISNUMBER(E278), E278, "")</f>
         <v>6</v>
       </c>
-      <c r="F288" t="str">
+      <c r="F288">
         <f t="shared" si="300"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G288">
         <f t="shared" si="300"/>
@@ -12521,9 +12553,9 @@
         <f t="shared" ref="E289:G289" si="301">IF(ISNUMBER(E279), E279, "")</f>
         <v>7</v>
       </c>
-      <c r="F289" t="str">
+      <c r="F289">
         <f t="shared" si="301"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G289">
         <f t="shared" si="301"/>
@@ -12563,9 +12595,9 @@
         <f t="shared" ref="E290:G290" si="302">IF(ISNUMBER(E280), E280, "")</f>
         <v>8</v>
       </c>
-      <c r="F290" t="str">
+      <c r="F290">
         <f t="shared" si="302"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G290">
         <f t="shared" si="302"/>
@@ -12605,9 +12637,9 @@
         <f t="shared" ref="E291:G291" si="303">IF(ISNUMBER(E281), E281, "")</f>
         <v>9</v>
       </c>
-      <c r="F291" t="str">
+      <c r="F291">
         <f t="shared" si="303"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G291">
         <f t="shared" si="303"/>
@@ -12689,9 +12721,9 @@
         <f t="shared" ref="E293:G293" si="305">IF(ISNUMBER(E283), E283, "")</f>
         <v>1</v>
       </c>
-      <c r="F293" t="str">
+      <c r="F293">
         <f t="shared" si="305"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G293">
         <f t="shared" si="305"/>
@@ -12731,9 +12763,9 @@
         <f t="shared" ref="E294:G294" si="306">IF(ISNUMBER(E284), E284, "")</f>
         <v>2</v>
       </c>
-      <c r="F294" t="str">
+      <c r="F294">
         <f t="shared" si="306"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G294">
         <f t="shared" si="306"/>
@@ -12773,9 +12805,9 @@
         <f t="shared" ref="E295:G295" si="307">IF(ISNUMBER(E285), E285, "")</f>
         <v>3</v>
       </c>
-      <c r="F295" t="str">
+      <c r="F295">
         <f t="shared" si="307"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G295">
         <f t="shared" si="307"/>
@@ -12815,9 +12847,9 @@
         <f t="shared" ref="E296:G296" si="308">IF(ISNUMBER(E286), E286, "")</f>
         <v>4</v>
       </c>
-      <c r="F296" t="str">
+      <c r="F296">
         <f t="shared" si="308"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G296">
         <f t="shared" si="308"/>
@@ -12857,9 +12889,9 @@
         <f t="shared" ref="E297:G297" si="309">IF(ISNUMBER(E287), E287, "")</f>
         <v>5</v>
       </c>
-      <c r="F297" t="str">
+      <c r="F297">
         <f t="shared" si="309"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G297">
         <f t="shared" si="309"/>
@@ -12899,9 +12931,9 @@
         <f t="shared" ref="E298:G298" si="310">IF(ISNUMBER(E288), E288, "")</f>
         <v>6</v>
       </c>
-      <c r="F298" t="str">
+      <c r="F298">
         <f t="shared" si="310"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G298">
         <f t="shared" si="310"/>
@@ -12941,9 +12973,9 @@
         <f t="shared" ref="E299:G299" si="311">IF(ISNUMBER(E289), E289, "")</f>
         <v>7</v>
       </c>
-      <c r="F299" t="str">
+      <c r="F299">
         <f t="shared" si="311"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G299">
         <f t="shared" si="311"/>
@@ -12983,9 +13015,9 @@
         <f t="shared" ref="E300:G300" si="312">IF(ISNUMBER(E290), E290, "")</f>
         <v>8</v>
       </c>
-      <c r="F300" t="str">
+      <c r="F300">
         <f t="shared" si="312"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G300">
         <f t="shared" si="312"/>
@@ -13025,9 +13057,9 @@
         <f t="shared" ref="E301:G301" si="313">IF(ISNUMBER(E291), E291, "")</f>
         <v>9</v>
       </c>
-      <c r="F301" t="str">
+      <c r="F301">
         <f t="shared" si="313"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G301">
         <f t="shared" si="313"/>
@@ -13109,9 +13141,9 @@
         <f t="shared" ref="E303:G303" si="315">IF(ISNUMBER(E293), E293, "")</f>
         <v>1</v>
       </c>
-      <c r="F303" t="str">
+      <c r="F303">
         <f t="shared" si="315"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G303">
         <f t="shared" si="315"/>
@@ -13151,9 +13183,9 @@
         <f t="shared" ref="E304:G304" si="316">IF(ISNUMBER(E294), E294, "")</f>
         <v>2</v>
       </c>
-      <c r="F304" t="str">
+      <c r="F304">
         <f t="shared" si="316"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G304">
         <f t="shared" si="316"/>
@@ -13193,9 +13225,9 @@
         <f t="shared" ref="E305:G305" si="317">IF(ISNUMBER(E295), E295, "")</f>
         <v>3</v>
       </c>
-      <c r="F305" t="str">
+      <c r="F305">
         <f t="shared" si="317"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G305">
         <f t="shared" si="317"/>
@@ -13235,9 +13267,9 @@
         <f t="shared" ref="E306:G306" si="318">IF(ISNUMBER(E296), E296, "")</f>
         <v>4</v>
       </c>
-      <c r="F306" t="str">
+      <c r="F306">
         <f t="shared" si="318"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G306">
         <f t="shared" si="318"/>
@@ -13277,9 +13309,9 @@
         <f t="shared" ref="E307:G307" si="319">IF(ISNUMBER(E297), E297, "")</f>
         <v>5</v>
       </c>
-      <c r="F307" t="str">
+      <c r="F307">
         <f t="shared" si="319"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G307">
         <f t="shared" si="319"/>
@@ -13319,9 +13351,9 @@
         <f t="shared" ref="E308:G308" si="320">IF(ISNUMBER(E298), E298, "")</f>
         <v>6</v>
       </c>
-      <c r="F308" t="str">
+      <c r="F308">
         <f t="shared" si="320"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G308">
         <f t="shared" si="320"/>
@@ -13361,9 +13393,9 @@
         <f t="shared" ref="E309:G309" si="321">IF(ISNUMBER(E299), E299, "")</f>
         <v>7</v>
       </c>
-      <c r="F309" t="str">
+      <c r="F309">
         <f t="shared" si="321"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G309">
         <f t="shared" si="321"/>
@@ -13403,9 +13435,9 @@
         <f t="shared" ref="E310:G310" si="322">IF(ISNUMBER(E300), E300, "")</f>
         <v>8</v>
       </c>
-      <c r="F310" t="str">
+      <c r="F310">
         <f t="shared" si="322"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G310">
         <f t="shared" si="322"/>
@@ -13445,9 +13477,9 @@
         <f t="shared" ref="E311:G311" si="323">IF(ISNUMBER(E301), E301, "")</f>
         <v>9</v>
       </c>
-      <c r="F311" t="str">
+      <c r="F311">
         <f t="shared" si="323"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G311">
         <f t="shared" si="323"/>
@@ -13529,9 +13561,9 @@
         <f t="shared" ref="E313:G313" si="325">IF(ISNUMBER(E303), E303, "")</f>
         <v>1</v>
       </c>
-      <c r="F313" t="str">
+      <c r="F313">
         <f t="shared" si="325"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G313">
         <f t="shared" si="325"/>
@@ -13571,9 +13603,9 @@
         <f t="shared" ref="E314:G314" si="326">IF(ISNUMBER(E304), E304, "")</f>
         <v>2</v>
       </c>
-      <c r="F314" t="str">
+      <c r="F314">
         <f t="shared" si="326"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G314">
         <f t="shared" si="326"/>
@@ -13613,9 +13645,9 @@
         <f t="shared" ref="E315:G315" si="327">IF(ISNUMBER(E305), E305, "")</f>
         <v>3</v>
       </c>
-      <c r="F315" t="str">
+      <c r="F315">
         <f t="shared" si="327"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G315">
         <f t="shared" si="327"/>
@@ -13655,9 +13687,9 @@
         <f t="shared" ref="E316:G316" si="328">IF(ISNUMBER(E306), E306, "")</f>
         <v>4</v>
       </c>
-      <c r="F316" t="str">
+      <c r="F316">
         <f t="shared" si="328"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G316">
         <f t="shared" si="328"/>
@@ -13697,9 +13729,9 @@
         <f t="shared" ref="E317:G317" si="329">IF(ISNUMBER(E307), E307, "")</f>
         <v>5</v>
       </c>
-      <c r="F317" t="str">
+      <c r="F317">
         <f t="shared" si="329"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G317">
         <f t="shared" si="329"/>
@@ -13739,9 +13771,9 @@
         <f t="shared" ref="E318:G318" si="330">IF(ISNUMBER(E308), E308, "")</f>
         <v>6</v>
       </c>
-      <c r="F318" t="str">
+      <c r="F318">
         <f t="shared" si="330"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G318">
         <f t="shared" si="330"/>
@@ -13781,9 +13813,9 @@
         <f t="shared" ref="E319:G319" si="331">IF(ISNUMBER(E309), E309, "")</f>
         <v>7</v>
       </c>
-      <c r="F319" t="str">
+      <c r="F319">
         <f t="shared" si="331"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G319">
         <f t="shared" si="331"/>
@@ -13823,9 +13855,9 @@
         <f t="shared" ref="E320:G320" si="332">IF(ISNUMBER(E310), E310, "")</f>
         <v>8</v>
       </c>
-      <c r="F320" t="str">
+      <c r="F320">
         <f t="shared" si="332"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G320">
         <f t="shared" si="332"/>
@@ -13865,9 +13897,9 @@
         <f t="shared" ref="E321:G321" si="333">IF(ISNUMBER(E311), E311, "")</f>
         <v>9</v>
       </c>
-      <c r="F321" t="str">
+      <c r="F321">
         <f t="shared" si="333"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G321">
         <f t="shared" si="333"/>
@@ -13949,9 +13981,9 @@
         <f t="shared" ref="E323:G323" si="335">IF(ISNUMBER(E313), E313, "")</f>
         <v>1</v>
       </c>
-      <c r="F323" t="str">
+      <c r="F323">
         <f t="shared" si="335"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G323">
         <f t="shared" si="335"/>
@@ -13991,9 +14023,9 @@
         <f t="shared" ref="E324:G324" si="336">IF(ISNUMBER(E314), E314, "")</f>
         <v>2</v>
       </c>
-      <c r="F324" t="str">
+      <c r="F324">
         <f t="shared" si="336"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G324">
         <f t="shared" si="336"/>
@@ -14033,9 +14065,9 @@
         <f t="shared" ref="E325:G325" si="337">IF(ISNUMBER(E315), E315, "")</f>
         <v>3</v>
       </c>
-      <c r="F325" t="str">
+      <c r="F325">
         <f t="shared" si="337"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G325">
         <f t="shared" si="337"/>
@@ -14075,9 +14107,9 @@
         <f t="shared" ref="E326:G326" si="338">IF(ISNUMBER(E316), E316, "")</f>
         <v>4</v>
       </c>
-      <c r="F326" t="str">
+      <c r="F326">
         <f t="shared" si="338"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G326">
         <f t="shared" si="338"/>
@@ -14117,9 +14149,9 @@
         <f t="shared" ref="E327:G327" si="339">IF(ISNUMBER(E317), E317, "")</f>
         <v>5</v>
       </c>
-      <c r="F327" t="str">
+      <c r="F327">
         <f t="shared" si="339"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G327">
         <f t="shared" si="339"/>
@@ -14159,9 +14191,9 @@
         <f t="shared" ref="E328:G328" si="340">IF(ISNUMBER(E318), E318, "")</f>
         <v>6</v>
       </c>
-      <c r="F328" t="str">
+      <c r="F328">
         <f t="shared" si="340"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G328">
         <f t="shared" si="340"/>
@@ -14201,9 +14233,9 @@
         <f t="shared" ref="E329:G329" si="341">IF(ISNUMBER(E319), E319, "")</f>
         <v>7</v>
       </c>
-      <c r="F329" t="str">
+      <c r="F329">
         <f t="shared" si="341"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G329">
         <f t="shared" si="341"/>
@@ -14243,9 +14275,9 @@
         <f t="shared" ref="E330:G330" si="342">IF(ISNUMBER(E320), E320, "")</f>
         <v>8</v>
       </c>
-      <c r="F330" t="str">
+      <c r="F330">
         <f t="shared" si="342"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G330">
         <f t="shared" si="342"/>
@@ -14285,9 +14317,9 @@
         <f t="shared" ref="E331:G331" si="343">IF(ISNUMBER(E321), E321, "")</f>
         <v>9</v>
       </c>
-      <c r="F331" t="str">
+      <c r="F331">
         <f t="shared" si="343"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G331">
         <f t="shared" si="343"/>
@@ -14369,9 +14401,9 @@
         <f t="shared" ref="E333:G333" si="347">IF(ISNUMBER(E323), E323, "")</f>
         <v>1</v>
       </c>
-      <c r="F333" t="str">
+      <c r="F333">
         <f t="shared" si="347"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G333">
         <f t="shared" si="347"/>
@@ -14411,9 +14443,9 @@
         <f t="shared" ref="E334:G334" si="349">IF(ISNUMBER(E324), E324, "")</f>
         <v>2</v>
       </c>
-      <c r="F334" t="str">
+      <c r="F334">
         <f t="shared" si="349"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G334">
         <f t="shared" si="349"/>
@@ -14453,9 +14485,9 @@
         <f t="shared" ref="E335:G335" si="352">IF(ISNUMBER(E325), E325, "")</f>
         <v>3</v>
       </c>
-      <c r="F335" t="str">
+      <c r="F335">
         <f t="shared" si="352"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G335">
         <f t="shared" si="352"/>
@@ -14495,9 +14527,9 @@
         <f t="shared" ref="E336:G336" si="353">IF(ISNUMBER(E326), E326, "")</f>
         <v>4</v>
       </c>
-      <c r="F336" t="str">
+      <c r="F336">
         <f t="shared" si="353"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G336">
         <f t="shared" si="353"/>
@@ -14537,9 +14569,9 @@
         <f t="shared" ref="E337:G337" si="354">IF(ISNUMBER(E327), E327, "")</f>
         <v>5</v>
       </c>
-      <c r="F337" t="str">
+      <c r="F337">
         <f t="shared" si="354"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G337">
         <f t="shared" si="354"/>
@@ -14579,9 +14611,9 @@
         <f t="shared" ref="E338:G338" si="355">IF(ISNUMBER(E328), E328, "")</f>
         <v>6</v>
       </c>
-      <c r="F338" t="str">
+      <c r="F338">
         <f t="shared" si="355"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G338">
         <f t="shared" si="355"/>
@@ -14621,9 +14653,9 @@
         <f t="shared" ref="E339:G339" si="356">IF(ISNUMBER(E329), E329, "")</f>
         <v>7</v>
       </c>
-      <c r="F339" t="str">
+      <c r="F339">
         <f t="shared" si="356"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G339">
         <f t="shared" si="356"/>
@@ -14663,9 +14695,9 @@
         <f t="shared" ref="E340:G340" si="357">IF(ISNUMBER(E330), E330, "")</f>
         <v>8</v>
       </c>
-      <c r="F340" t="str">
+      <c r="F340">
         <f t="shared" si="357"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G340">
         <f t="shared" si="357"/>
@@ -14705,9 +14737,9 @@
         <f t="shared" ref="E341:G341" si="358">IF(ISNUMBER(E331), E331, "")</f>
         <v>9</v>
       </c>
-      <c r="F341" t="str">
+      <c r="F341">
         <f t="shared" si="358"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G341">
         <f t="shared" si="358"/>
@@ -14789,9 +14821,9 @@
         <f t="shared" ref="E343:G343" si="360">IF(ISNUMBER(E333), E333, "")</f>
         <v>1</v>
       </c>
-      <c r="F343" t="str">
+      <c r="F343">
         <f t="shared" si="360"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G343">
         <f t="shared" si="360"/>
@@ -14831,9 +14863,9 @@
         <f t="shared" ref="E344:G344" si="361">IF(ISNUMBER(E334), E334, "")</f>
         <v>2</v>
       </c>
-      <c r="F344" t="str">
+      <c r="F344">
         <f t="shared" si="361"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G344">
         <f t="shared" si="361"/>
@@ -14873,9 +14905,9 @@
         <f t="shared" ref="E345:G345" si="362">IF(ISNUMBER(E335), E335, "")</f>
         <v>3</v>
       </c>
-      <c r="F345" t="str">
+      <c r="F345">
         <f t="shared" si="362"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G345">
         <f t="shared" si="362"/>
@@ -14915,9 +14947,9 @@
         <f t="shared" ref="E346:G346" si="363">IF(ISNUMBER(E336), E336, "")</f>
         <v>4</v>
       </c>
-      <c r="F346" t="str">
+      <c r="F346">
         <f t="shared" si="363"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G346">
         <f t="shared" si="363"/>
@@ -14957,9 +14989,9 @@
         <f t="shared" ref="E347:G347" si="364">IF(ISNUMBER(E337), E337, "")</f>
         <v>5</v>
       </c>
-      <c r="F347" t="str">
+      <c r="F347">
         <f t="shared" si="364"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G347">
         <f t="shared" si="364"/>
@@ -14999,9 +15031,9 @@
         <f t="shared" ref="E348:G348" si="365">IF(ISNUMBER(E338), E338, "")</f>
         <v>6</v>
       </c>
-      <c r="F348" t="str">
+      <c r="F348">
         <f t="shared" si="365"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G348">
         <f t="shared" si="365"/>
@@ -15041,9 +15073,9 @@
         <f t="shared" ref="E349:G349" si="366">IF(ISNUMBER(E339), E339, "")</f>
         <v>7</v>
       </c>
-      <c r="F349" t="str">
+      <c r="F349">
         <f t="shared" si="366"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G349">
         <f t="shared" si="366"/>
@@ -15083,9 +15115,9 @@
         <f t="shared" ref="E350:G350" si="367">IF(ISNUMBER(E340), E340, "")</f>
         <v>8</v>
       </c>
-      <c r="F350" t="str">
+      <c r="F350">
         <f t="shared" si="367"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G350">
         <f t="shared" si="367"/>
@@ -15125,9 +15157,9 @@
         <f t="shared" ref="E351:G351" si="368">IF(ISNUMBER(E341), E341, "")</f>
         <v>9</v>
       </c>
-      <c r="F351" t="str">
+      <c r="F351">
         <f t="shared" si="368"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G351">
         <f t="shared" si="368"/>
@@ -15209,9 +15241,9 @@
         <f t="shared" ref="E353:G353" si="370">IF(ISNUMBER(E343), E343, "")</f>
         <v>1</v>
       </c>
-      <c r="F353" t="str">
+      <c r="F353">
         <f t="shared" si="370"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G353">
         <f t="shared" si="370"/>
@@ -15251,9 +15283,9 @@
         <f t="shared" ref="E354:G354" si="371">IF(ISNUMBER(E344), E344, "")</f>
         <v>2</v>
       </c>
-      <c r="F354" t="str">
+      <c r="F354">
         <f t="shared" si="371"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G354">
         <f t="shared" si="371"/>
@@ -15293,9 +15325,9 @@
         <f t="shared" ref="E355:G355" si="372">IF(ISNUMBER(E345), E345, "")</f>
         <v>3</v>
       </c>
-      <c r="F355" t="str">
+      <c r="F355">
         <f t="shared" si="372"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G355">
         <f t="shared" si="372"/>
@@ -15335,9 +15367,9 @@
         <f t="shared" ref="E356:G356" si="373">IF(ISNUMBER(E346), E346, "")</f>
         <v>4</v>
       </c>
-      <c r="F356" t="str">
+      <c r="F356">
         <f t="shared" si="373"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G356">
         <f t="shared" si="373"/>
@@ -15377,9 +15409,9 @@
         <f t="shared" ref="E357:G357" si="374">IF(ISNUMBER(E347), E347, "")</f>
         <v>5</v>
       </c>
-      <c r="F357" t="str">
+      <c r="F357">
         <f t="shared" si="374"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G357">
         <f t="shared" si="374"/>
@@ -15419,9 +15451,9 @@
         <f t="shared" ref="E358:G358" si="375">IF(ISNUMBER(E348), E348, "")</f>
         <v>6</v>
       </c>
-      <c r="F358" t="str">
+      <c r="F358">
         <f t="shared" si="375"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G358">
         <f t="shared" si="375"/>
@@ -15461,9 +15493,9 @@
         <f t="shared" ref="E359:G359" si="376">IF(ISNUMBER(E349), E349, "")</f>
         <v>7</v>
       </c>
-      <c r="F359" t="str">
+      <c r="F359">
         <f t="shared" si="376"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G359">
         <f t="shared" si="376"/>
@@ -15503,9 +15535,9 @@
         <f t="shared" ref="E360:G360" si="377">IF(ISNUMBER(E350), E350, "")</f>
         <v>8</v>
       </c>
-      <c r="F360" t="str">
+      <c r="F360">
         <f t="shared" si="377"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G360">
         <f t="shared" si="377"/>
@@ -15545,9 +15577,9 @@
         <f t="shared" ref="E361:G361" si="378">IF(ISNUMBER(E351), E351, "")</f>
         <v>9</v>
       </c>
-      <c r="F361" t="str">
+      <c r="F361">
         <f t="shared" si="378"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G361">
         <f t="shared" si="378"/>
@@ -15629,9 +15661,9 @@
         <f t="shared" ref="E363:G363" si="380">IF(ISNUMBER(E353), E353, "")</f>
         <v>1</v>
       </c>
-      <c r="F363" t="str">
+      <c r="F363">
         <f t="shared" si="380"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G363">
         <f t="shared" si="380"/>
@@ -15671,9 +15703,9 @@
         <f t="shared" ref="E364:G364" si="381">IF(ISNUMBER(E354), E354, "")</f>
         <v>2</v>
       </c>
-      <c r="F364" t="str">
+      <c r="F364">
         <f t="shared" si="381"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G364">
         <f t="shared" si="381"/>
@@ -15713,9 +15745,9 @@
         <f t="shared" ref="E365:G365" si="382">IF(ISNUMBER(E355), E355, "")</f>
         <v>3</v>
       </c>
-      <c r="F365" t="str">
+      <c r="F365">
         <f t="shared" si="382"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G365">
         <f t="shared" si="382"/>
@@ -15755,9 +15787,9 @@
         <f t="shared" ref="E366:G366" si="383">IF(ISNUMBER(E356), E356, "")</f>
         <v>4</v>
       </c>
-      <c r="F366" t="str">
+      <c r="F366">
         <f t="shared" si="383"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G366">
         <f t="shared" si="383"/>
@@ -15797,9 +15829,9 @@
         <f t="shared" ref="E367:G367" si="384">IF(ISNUMBER(E357), E357, "")</f>
         <v>5</v>
       </c>
-      <c r="F367" t="str">
+      <c r="F367">
         <f t="shared" si="384"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G367">
         <f t="shared" si="384"/>
@@ -15839,9 +15871,9 @@
         <f t="shared" ref="E368:G368" si="385">IF(ISNUMBER(E358), E358, "")</f>
         <v>6</v>
       </c>
-      <c r="F368" t="str">
+      <c r="F368">
         <f t="shared" si="385"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G368">
         <f t="shared" si="385"/>
@@ -15881,9 +15913,9 @@
         <f t="shared" ref="E369:G369" si="386">IF(ISNUMBER(E359), E359, "")</f>
         <v>7</v>
       </c>
-      <c r="F369" t="str">
+      <c r="F369">
         <f t="shared" si="386"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G369">
         <f t="shared" si="386"/>
@@ -15923,9 +15955,9 @@
         <f t="shared" ref="E370:G370" si="387">IF(ISNUMBER(E360), E360, "")</f>
         <v>8</v>
       </c>
-      <c r="F370" t="str">
+      <c r="F370">
         <f t="shared" si="387"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G370">
         <f t="shared" si="387"/>
@@ -15965,9 +15997,9 @@
         <f t="shared" ref="E371:G371" si="388">IF(ISNUMBER(E361), E361, "")</f>
         <v>9</v>
       </c>
-      <c r="F371" t="str">
+      <c r="F371">
         <f t="shared" si="388"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G371">
         <f t="shared" si="388"/>
@@ -16049,9 +16081,9 @@
         <f t="shared" ref="E373:G373" si="390">IF(ISNUMBER(E363), E363, "")</f>
         <v>1</v>
       </c>
-      <c r="F373" t="str">
+      <c r="F373">
         <f t="shared" si="390"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G373">
         <f t="shared" si="390"/>
@@ -16091,9 +16123,9 @@
         <f t="shared" ref="E374:G374" si="391">IF(ISNUMBER(E364), E364, "")</f>
         <v>2</v>
       </c>
-      <c r="F374" t="str">
+      <c r="F374">
         <f t="shared" si="391"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G374">
         <f t="shared" si="391"/>
@@ -16133,9 +16165,9 @@
         <f t="shared" ref="E375:G375" si="392">IF(ISNUMBER(E365), E365, "")</f>
         <v>3</v>
       </c>
-      <c r="F375" t="str">
+      <c r="F375">
         <f t="shared" si="392"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G375">
         <f t="shared" si="392"/>
@@ -16175,9 +16207,9 @@
         <f t="shared" ref="E376:G376" si="393">IF(ISNUMBER(E366), E366, "")</f>
         <v>4</v>
       </c>
-      <c r="F376" t="str">
+      <c r="F376">
         <f t="shared" si="393"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G376">
         <f t="shared" si="393"/>
@@ -16217,9 +16249,9 @@
         <f t="shared" ref="E377:G377" si="394">IF(ISNUMBER(E367), E367, "")</f>
         <v>5</v>
       </c>
-      <c r="F377" t="str">
+      <c r="F377">
         <f t="shared" si="394"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G377">
         <f t="shared" si="394"/>
@@ -16259,9 +16291,9 @@
         <f t="shared" ref="E378:G378" si="395">IF(ISNUMBER(E368), E368, "")</f>
         <v>6</v>
       </c>
-      <c r="F378" t="str">
+      <c r="F378">
         <f t="shared" si="395"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G378">
         <f t="shared" si="395"/>
@@ -16301,9 +16333,9 @@
         <f t="shared" ref="E379:G379" si="396">IF(ISNUMBER(E369), E369, "")</f>
         <v>7</v>
       </c>
-      <c r="F379" t="str">
+      <c r="F379">
         <f t="shared" si="396"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G379">
         <f t="shared" si="396"/>
@@ -16343,9 +16375,9 @@
         <f t="shared" ref="E380:G380" si="397">IF(ISNUMBER(E370), E370, "")</f>
         <v>8</v>
       </c>
-      <c r="F380" t="str">
+      <c r="F380">
         <f t="shared" si="397"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G380">
         <f t="shared" si="397"/>
@@ -16385,9 +16417,9 @@
         <f t="shared" ref="E381:G381" si="398">IF(ISNUMBER(E371), E371, "")</f>
         <v>9</v>
       </c>
-      <c r="F381" t="str">
+      <c r="F381">
         <f t="shared" si="398"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G381">
         <f t="shared" si="398"/>
@@ -16469,9 +16501,9 @@
         <f t="shared" ref="E383:G383" si="400">IF(ISNUMBER(E373), E373, "")</f>
         <v>1</v>
       </c>
-      <c r="F383" t="str">
+      <c r="F383">
         <f t="shared" si="400"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G383">
         <f t="shared" si="400"/>
@@ -16511,9 +16543,9 @@
         <f t="shared" ref="E384:G384" si="401">IF(ISNUMBER(E374), E374, "")</f>
         <v>2</v>
       </c>
-      <c r="F384" t="str">
+      <c r="F384">
         <f t="shared" si="401"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G384">
         <f t="shared" si="401"/>
@@ -16553,9 +16585,9 @@
         <f t="shared" ref="E385:G385" si="402">IF(ISNUMBER(E375), E375, "")</f>
         <v>3</v>
       </c>
-      <c r="F385" t="str">
+      <c r="F385">
         <f t="shared" si="402"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G385">
         <f t="shared" si="402"/>
@@ -16595,9 +16627,9 @@
         <f t="shared" ref="E386:G386" si="403">IF(ISNUMBER(E376), E376, "")</f>
         <v>4</v>
       </c>
-      <c r="F386" t="str">
+      <c r="F386">
         <f t="shared" si="403"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G386">
         <f t="shared" si="403"/>
@@ -16637,9 +16669,9 @@
         <f t="shared" ref="E387:G387" si="404">IF(ISNUMBER(E377), E377, "")</f>
         <v>5</v>
       </c>
-      <c r="F387" t="str">
+      <c r="F387">
         <f t="shared" si="404"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G387">
         <f t="shared" si="404"/>
@@ -16679,9 +16711,9 @@
         <f t="shared" ref="E388:G388" si="405">IF(ISNUMBER(E378), E378, "")</f>
         <v>6</v>
       </c>
-      <c r="F388" t="str">
+      <c r="F388">
         <f t="shared" si="405"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G388">
         <f t="shared" si="405"/>
@@ -16721,9 +16753,9 @@
         <f t="shared" ref="E389:G389" si="406">IF(ISNUMBER(E379), E379, "")</f>
         <v>7</v>
       </c>
-      <c r="F389" t="str">
+      <c r="F389">
         <f t="shared" si="406"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G389">
         <f t="shared" si="406"/>
@@ -16763,9 +16795,9 @@
         <f t="shared" ref="E390:G390" si="407">IF(ISNUMBER(E380), E380, "")</f>
         <v>8</v>
       </c>
-      <c r="F390" t="str">
+      <c r="F390">
         <f t="shared" si="407"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G390">
         <f t="shared" si="407"/>
@@ -16805,9 +16837,9 @@
         <f t="shared" ref="E391:G391" si="408">IF(ISNUMBER(E381), E381, "")</f>
         <v>9</v>
       </c>
-      <c r="F391" t="str">
+      <c r="F391">
         <f t="shared" si="408"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G391">
         <f t="shared" si="408"/>
@@ -16889,9 +16921,9 @@
         <f t="shared" ref="E393:G393" si="410">IF(ISNUMBER(E383), E383, "")</f>
         <v>1</v>
       </c>
-      <c r="F393" t="str">
+      <c r="F393">
         <f t="shared" si="410"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G393">
         <f t="shared" si="410"/>
@@ -16931,9 +16963,9 @@
         <f t="shared" ref="E394:G394" si="411">IF(ISNUMBER(E384), E384, "")</f>
         <v>2</v>
       </c>
-      <c r="F394" t="str">
+      <c r="F394">
         <f t="shared" si="411"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G394">
         <f t="shared" si="411"/>
@@ -16973,9 +17005,9 @@
         <f t="shared" ref="E395:G395" si="412">IF(ISNUMBER(E385), E385, "")</f>
         <v>3</v>
       </c>
-      <c r="F395" t="str">
+      <c r="F395">
         <f t="shared" si="412"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G395">
         <f t="shared" si="412"/>
@@ -17015,9 +17047,9 @@
         <f t="shared" ref="E396:G396" si="413">IF(ISNUMBER(E386), E386, "")</f>
         <v>4</v>
       </c>
-      <c r="F396" t="str">
+      <c r="F396">
         <f t="shared" si="413"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="G396">
         <f t="shared" si="413"/>
@@ -17057,9 +17089,9 @@
         <f t="shared" ref="E397:G397" si="416">IF(ISNUMBER(E387), E387, "")</f>
         <v>5</v>
       </c>
-      <c r="F397" t="str">
+      <c r="F397">
         <f t="shared" si="416"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G397">
         <f t="shared" si="416"/>
@@ -17099,9 +17131,9 @@
         <f t="shared" ref="E398:G398" si="418">IF(ISNUMBER(E388), E388, "")</f>
         <v>6</v>
       </c>
-      <c r="F398" t="str">
+      <c r="F398">
         <f t="shared" si="418"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="G398">
         <f t="shared" si="418"/>
@@ -17141,9 +17173,9 @@
         <f t="shared" ref="E399:G399" si="421">IF(ISNUMBER(E389), E389, "")</f>
         <v>7</v>
       </c>
-      <c r="F399" t="str">
+      <c r="F399">
         <f t="shared" si="421"/>
-        <v/>
+        <v>7</v>
       </c>
       <c r="G399">
         <f t="shared" si="421"/>
@@ -17183,9 +17215,9 @@
         <f t="shared" ref="E400:G400" si="422">IF(ISNUMBER(E390), E390, "")</f>
         <v>8</v>
       </c>
-      <c r="F400" t="str">
+      <c r="F400">
         <f t="shared" si="422"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="G400">
         <f t="shared" si="422"/>
@@ -17225,9 +17257,9 @@
         <f t="shared" ref="E401:G401" si="423">IF(ISNUMBER(E391), E391, "")</f>
         <v>9</v>
       </c>
-      <c r="F401" t="str">
+      <c r="F401">
         <f t="shared" si="423"/>
-        <v/>
+        <v>9</v>
       </c>
       <c r="G401">
         <f t="shared" si="423"/>
@@ -17293,7 +17325,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>